<commit_message>
pipeline: Move one status field to correct place
</commit_message>
<xml_diff>
--- a/indigo/spreadsheetform_guides/pipeline_v001.xlsx
+++ b/indigo/spreadsheetform_guides/pipeline_v001.xlsx
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="899" uniqueCount="707">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="900" uniqueCount="707">
   <si>
     <t xml:space="preserve">INDIGO Pipeline ID</t>
   </si>
@@ -6815,15 +6815,17 @@
       </c>
       <c r="E118" s="12"/>
     </row>
-    <row r="119" customFormat="false" ht="29.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="119" customFormat="false" ht="44.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A119" s="4"/>
       <c r="B119" s="4" t="s">
         <v>14</v>
       </c>
       <c r="C119" s="7" t="s">
+        <v>41</v>
+      </c>
+      <c r="D119" s="7" t="s">
         <v>181</v>
       </c>
-      <c r="D119" s="7"/>
       <c r="E119" s="12"/>
     </row>
     <row r="120" customFormat="false" ht="44" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -7046,7 +7048,7 @@
       <formula1>0</formula1>
       <formula2>0</formula2>
     </dataValidation>
-    <dataValidation allowBlank="true" operator="equal" showDropDown="false" showErrorMessage="true" showInputMessage="false" sqref="D108:D119" type="none">
+    <dataValidation allowBlank="true" operator="equal" showDropDown="false" showErrorMessage="true" showInputMessage="false" sqref="D108:D118 C119" type="none">
       <formula1>0</formula1>
       <formula2>0</formula2>
     </dataValidation>

</xml_diff>

<commit_message>
pipeline: Add drop downs to spreadsheet
</commit_message>
<xml_diff>
--- a/indigo/spreadsheetform_guides/pipeline_v001.xlsx
+++ b/indigo/spreadsheetform_guides/pipeline_v001.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="1"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="0"/>
   </bookViews>
   <sheets>
     <sheet name="Introduction" sheetId="1" state="visible" r:id="rId2"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="900" uniqueCount="707">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="865" uniqueCount="701">
   <si>
     <t xml:space="preserve">INDIGO Pipeline ID</t>
   </si>
@@ -105,9 +105,6 @@
     <t xml:space="preserve">SPREADSHEETFORM:SINGLE:state_development/state/status</t>
   </si>
   <si>
-    <t xml:space="preserve">OPTIONS:Current, Abandoned, Launched</t>
-  </si>
-  <si>
     <t xml:space="preserve">Reason for abandoned</t>
   </si>
   <si>
@@ -138,12 +135,6 @@
     <t xml:space="preserve">SPREADSHEETFORM:SINGLE:stage_development/stage/status</t>
   </si>
   <si>
-    <t xml:space="preserve">OPTIONS: Scoping (e.g. pre-feasibility study to support market mapping and issue identification).   Early stage (e.g. beginning a feasibility study).  Late stage (e.g. final deal construction and placement) .Final negotiations. Abandoned.  Successful </t>
-  </si>
-  <si>
-    <t xml:space="preserve">Scoping (e.g. pre-feasibility study to support market mapping and issue identification)  </t>
-  </si>
-  <si>
     <t xml:space="preserve">SPREADSHEETFORM:SINGLE:stage_development/source_ids</t>
   </si>
   <si>
@@ -160,9 +151,6 @@
   </si>
   <si>
     <t xml:space="preserve">-</t>
-  </si>
-  <si>
-    <t xml:space="preserve">OPTIONS: Yes, No</t>
   </si>
   <si>
     <t xml:space="preserve">Outcomes Fund</t>
@@ -248,9 +236,6 @@
     <t xml:space="preserve">SPREADSHEETFORM:SINGLE:dates/expected_launch_date/status</t>
   </si>
   <si>
-    <t xml:space="preserve">OPTIONS: Q1 – 2022,  Q2 – 2022, Q3 – 2022, Q4 – 2022, Q1 - 2023 ,Q2 – 2023,  Don’t Know </t>
-  </si>
-  <si>
     <t xml:space="preserve">Total expected project development time</t>
   </si>
   <si>
@@ -258,9 +243,6 @@
   </si>
   <si>
     <t xml:space="preserve">SPREADSHEETFORM:SINGLE:dates/expected_development_time/status</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Options  0-6 months, 6-12 months, 12-24 months, &gt;24 months </t>
   </si>
   <si>
     <t xml:space="preserve">Expected length of project (years)</t>
@@ -2500,8 +2482,8 @@
   </sheetPr>
   <dimension ref="A2:C10"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="91" zoomScaleNormal="91" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A11" activeCellId="0" sqref="A11"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="91" zoomScaleNormal="91" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -2568,47 +2550,47 @@
   <sheetData>
     <row r="1" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="12" t="s">
-        <v>351</v>
+        <v>345</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="12" t="s">
-        <v>352</v>
+        <v>346</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="46.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="12" t="s">
-        <v>353</v>
+        <v>347</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="68.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="12" t="s">
-        <v>354</v>
+        <v>348</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="12" t="s">
-        <v>355</v>
+        <v>349</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="12" t="s">
-        <v>356</v>
+        <v>350</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="68.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="12" t="s">
-        <v>357</v>
+        <v>351</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="12" t="s">
-        <v>358</v>
+        <v>352</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="12" t="s">
-        <v>359</v>
+        <v>353</v>
       </c>
     </row>
   </sheetData>
@@ -2652,26 +2634,26 @@
       <c r="B2" s="4"/>
       <c r="C2" s="4"/>
       <c r="D2" s="4" t="s">
-        <v>216</v>
+        <v>210</v>
       </c>
       <c r="E2" s="4"/>
       <c r="F2" s="4"/>
     </row>
     <row r="3" customFormat="false" ht="30" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="14" t="s">
-        <v>283</v>
+        <v>277</v>
       </c>
       <c r="B3" s="9" t="s">
-        <v>284</v>
+        <v>278</v>
       </c>
       <c r="C3" s="9" t="s">
-        <v>360</v>
+        <v>354</v>
       </c>
       <c r="D3" s="14" t="s">
-        <v>218</v>
+        <v>212</v>
       </c>
       <c r="E3" s="4" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="F3" s="4" t="s">
         <v>14</v>
@@ -2679,22 +2661,22 @@
     </row>
     <row r="4" customFormat="false" ht="87" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="15" t="s">
-        <v>361</v>
+        <v>355</v>
       </c>
       <c r="B4" s="7" t="s">
-        <v>362</v>
+        <v>356</v>
       </c>
       <c r="C4" s="7" t="s">
-        <v>363</v>
+        <v>357</v>
       </c>
       <c r="D4" s="15" t="s">
-        <v>364</v>
+        <v>358</v>
       </c>
       <c r="E4" s="7" t="s">
-        <v>365</v>
+        <v>359</v>
       </c>
       <c r="F4" s="7" t="s">
-        <v>366</v>
+        <v>360</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3002,62 +2984,62 @@
       <c r="N2" s="4"/>
       <c r="O2" s="4"/>
       <c r="P2" s="4" t="s">
-        <v>216</v>
+        <v>210</v>
       </c>
       <c r="Q2" s="4"/>
       <c r="R2" s="4"/>
     </row>
     <row r="3" customFormat="false" ht="58.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="16" t="s">
-        <v>282</v>
+        <v>276</v>
       </c>
       <c r="B3" s="9" t="s">
+        <v>361</v>
+      </c>
+      <c r="C3" s="9" t="s">
+        <v>362</v>
+      </c>
+      <c r="D3" s="9" t="s">
+        <v>363</v>
+      </c>
+      <c r="E3" s="9" t="s">
+        <v>364</v>
+      </c>
+      <c r="F3" s="9" t="s">
+        <v>365</v>
+      </c>
+      <c r="G3" s="4" t="s">
+        <v>366</v>
+      </c>
+      <c r="H3" s="9" t="s">
         <v>367</v>
       </c>
-      <c r="C3" s="9" t="s">
+      <c r="I3" s="9" t="s">
         <v>368</v>
       </c>
-      <c r="D3" s="9" t="s">
+      <c r="J3" s="9" t="s">
         <v>369</v>
       </c>
-      <c r="E3" s="9" t="s">
+      <c r="K3" s="9" t="s">
         <v>370</v>
       </c>
-      <c r="F3" s="9" t="s">
+      <c r="L3" s="9" t="s">
         <v>371</v>
       </c>
-      <c r="G3" s="4" t="s">
+      <c r="M3" s="9" t="s">
         <v>372</v>
       </c>
-      <c r="H3" s="9" t="s">
+      <c r="N3" s="9" t="s">
         <v>373</v>
       </c>
-      <c r="I3" s="9" t="s">
+      <c r="O3" s="9" t="s">
         <v>374</v>
       </c>
-      <c r="J3" s="9" t="s">
-        <v>375</v>
-      </c>
-      <c r="K3" s="9" t="s">
-        <v>376</v>
-      </c>
-      <c r="L3" s="9" t="s">
-        <v>377</v>
-      </c>
-      <c r="M3" s="9" t="s">
-        <v>378</v>
-      </c>
-      <c r="N3" s="9" t="s">
-        <v>379</v>
-      </c>
-      <c r="O3" s="9" t="s">
-        <v>380</v>
-      </c>
       <c r="P3" s="14" t="s">
-        <v>218</v>
+        <v>212</v>
       </c>
       <c r="Q3" s="4" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="R3" s="4" t="s">
         <v>14</v>
@@ -3065,58 +3047,58 @@
     </row>
     <row r="4" customFormat="false" ht="115.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="19" t="s">
+        <v>375</v>
+      </c>
+      <c r="B4" s="7" t="s">
+        <v>376</v>
+      </c>
+      <c r="C4" s="7" t="s">
+        <v>377</v>
+      </c>
+      <c r="D4" s="7" t="s">
+        <v>378</v>
+      </c>
+      <c r="E4" s="7" t="s">
+        <v>379</v>
+      </c>
+      <c r="F4" s="7" t="s">
+        <v>380</v>
+      </c>
+      <c r="G4" s="7" t="s">
         <v>381</v>
       </c>
-      <c r="B4" s="7" t="s">
+      <c r="H4" s="7" t="s">
         <v>382</v>
       </c>
-      <c r="C4" s="7" t="s">
+      <c r="I4" s="7" t="s">
         <v>383</v>
       </c>
-      <c r="D4" s="7" t="s">
+      <c r="J4" s="7" t="s">
         <v>384</v>
       </c>
-      <c r="E4" s="7" t="s">
+      <c r="K4" s="7" t="s">
         <v>385</v>
       </c>
-      <c r="F4" s="7" t="s">
+      <c r="L4" s="7" t="s">
         <v>386</v>
       </c>
-      <c r="G4" s="7" t="s">
+      <c r="M4" s="7" t="s">
         <v>387</v>
       </c>
-      <c r="H4" s="7" t="s">
+      <c r="N4" s="7" t="s">
         <v>388</v>
       </c>
-      <c r="I4" s="7" t="s">
+      <c r="O4" s="7" t="s">
         <v>389</v>
       </c>
-      <c r="J4" s="7" t="s">
+      <c r="P4" s="15" t="s">
         <v>390</v>
       </c>
-      <c r="K4" s="7" t="s">
+      <c r="Q4" s="7" t="s">
         <v>391</v>
       </c>
-      <c r="L4" s="7" t="s">
+      <c r="R4" s="7" t="s">
         <v>392</v>
-      </c>
-      <c r="M4" s="7" t="s">
-        <v>393</v>
-      </c>
-      <c r="N4" s="7" t="s">
-        <v>394</v>
-      </c>
-      <c r="O4" s="7" t="s">
-        <v>395</v>
-      </c>
-      <c r="P4" s="15" t="s">
-        <v>396</v>
-      </c>
-      <c r="Q4" s="7" t="s">
-        <v>397</v>
-      </c>
-      <c r="R4" s="7" t="s">
-        <v>398</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3738,277 +3720,277 @@
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="0" t="s">
-        <v>399</v>
+        <v>393</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="0" t="s">
-        <v>400</v>
+        <v>394</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="0" t="s">
-        <v>401</v>
+        <v>395</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="0" t="s">
-        <v>402</v>
+        <v>396</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="0" t="s">
-        <v>403</v>
+        <v>397</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="0" t="s">
-        <v>404</v>
+        <v>398</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="0" t="s">
-        <v>405</v>
+        <v>399</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="0" t="s">
-        <v>406</v>
+        <v>400</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="0" t="s">
-        <v>407</v>
+        <v>401</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="0" t="s">
-        <v>408</v>
+        <v>402</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="0" t="s">
-        <v>409</v>
+        <v>403</v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="0" t="s">
-        <v>410</v>
+        <v>404</v>
       </c>
     </row>
     <row r="15" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A15" s="0" t="s">
-        <v>411</v>
+        <v>405</v>
       </c>
     </row>
     <row r="16" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A16" s="0" t="s">
-        <v>412</v>
+        <v>406</v>
       </c>
     </row>
     <row r="17" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A17" s="0" t="s">
-        <v>413</v>
+        <v>407</v>
       </c>
     </row>
     <row r="18" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A18" s="0" t="s">
-        <v>414</v>
+        <v>408</v>
       </c>
     </row>
     <row r="19" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A19" s="0" t="s">
-        <v>415</v>
+        <v>409</v>
       </c>
     </row>
     <row r="20" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A20" s="0" t="s">
-        <v>416</v>
+        <v>410</v>
       </c>
     </row>
     <row r="21" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A21" s="0" t="s">
-        <v>417</v>
+        <v>411</v>
       </c>
     </row>
     <row r="22" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A22" s="0" t="s">
-        <v>418</v>
+        <v>412</v>
       </c>
     </row>
     <row r="23" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A23" s="0" t="s">
-        <v>419</v>
+        <v>413</v>
       </c>
     </row>
     <row r="24" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A24" s="0" t="s">
-        <v>420</v>
+        <v>414</v>
       </c>
     </row>
     <row r="25" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A25" s="0" t="s">
-        <v>421</v>
+        <v>415</v>
       </c>
     </row>
     <row r="26" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A26" s="0" t="s">
-        <v>422</v>
+        <v>416</v>
       </c>
     </row>
     <row r="27" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A27" s="0" t="s">
-        <v>423</v>
+        <v>417</v>
       </c>
     </row>
     <row r="28" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A28" s="0" t="s">
-        <v>424</v>
+        <v>418</v>
       </c>
     </row>
     <row r="29" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A29" s="0" t="s">
-        <v>425</v>
+        <v>419</v>
       </c>
     </row>
     <row r="30" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A30" s="0" t="s">
-        <v>426</v>
+        <v>420</v>
       </c>
     </row>
     <row r="31" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A31" s="0" t="s">
-        <v>427</v>
+        <v>421</v>
       </c>
     </row>
     <row r="32" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A32" s="0" t="s">
-        <v>428</v>
+        <v>422</v>
       </c>
     </row>
     <row r="33" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A33" s="0" t="s">
-        <v>429</v>
+        <v>423</v>
       </c>
     </row>
     <row r="34" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A34" s="0" t="s">
-        <v>430</v>
+        <v>424</v>
       </c>
     </row>
     <row r="35" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A35" s="0" t="s">
-        <v>431</v>
+        <v>425</v>
       </c>
     </row>
     <row r="36" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A36" s="0" t="s">
-        <v>432</v>
+        <v>426</v>
       </c>
     </row>
     <row r="37" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A37" s="0" t="s">
-        <v>433</v>
+        <v>427</v>
       </c>
     </row>
     <row r="38" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A38" s="0" t="s">
-        <v>434</v>
+        <v>428</v>
       </c>
     </row>
     <row r="39" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A39" s="0" t="s">
-        <v>435</v>
+        <v>429</v>
       </c>
     </row>
     <row r="40" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A40" s="0" t="s">
-        <v>436</v>
+        <v>430</v>
       </c>
     </row>
     <row r="41" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A41" s="0" t="s">
-        <v>437</v>
+        <v>431</v>
       </c>
     </row>
     <row r="42" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A42" s="0" t="s">
-        <v>438</v>
+        <v>432</v>
       </c>
     </row>
     <row r="43" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A43" s="0" t="s">
-        <v>439</v>
+        <v>433</v>
       </c>
     </row>
     <row r="44" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A44" s="0" t="s">
-        <v>440</v>
+        <v>434</v>
       </c>
     </row>
     <row r="45" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A45" s="0" t="s">
-        <v>441</v>
+        <v>435</v>
       </c>
     </row>
     <row r="46" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A46" s="0" t="s">
-        <v>442</v>
+        <v>436</v>
       </c>
     </row>
     <row r="47" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A47" s="0" t="s">
-        <v>443</v>
+        <v>437</v>
       </c>
     </row>
     <row r="48" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A48" s="0" t="s">
-        <v>444</v>
+        <v>438</v>
       </c>
     </row>
     <row r="49" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A49" s="0" t="s">
-        <v>445</v>
+        <v>439</v>
       </c>
     </row>
     <row r="50" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A50" s="0" t="s">
-        <v>446</v>
+        <v>440</v>
       </c>
     </row>
     <row r="51" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A51" s="0" t="s">
-        <v>447</v>
+        <v>441</v>
       </c>
     </row>
     <row r="52" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A52" s="0" t="s">
-        <v>448</v>
+        <v>442</v>
       </c>
     </row>
     <row r="53" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A53" s="0" t="s">
-        <v>449</v>
+        <v>443</v>
       </c>
     </row>
     <row r="54" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A54" s="0" t="s">
-        <v>450</v>
+        <v>444</v>
       </c>
     </row>
     <row r="55" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A55" s="0" t="s">
-        <v>451</v>
+        <v>445</v>
       </c>
     </row>
     <row r="56" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A56" s="0" t="s">
-        <v>452</v>
+        <v>446</v>
       </c>
     </row>
     <row r="57" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A57" s="0" t="s">
-        <v>453</v>
+        <v>447</v>
       </c>
     </row>
   </sheetData>
@@ -4030,7 +4012,7 @@
   <dimension ref="A2:D32"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C6" activeCellId="0" sqref="C6"/>
+      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -4044,19 +4026,19 @@
       <c r="A2" s="4"/>
       <c r="B2" s="4"/>
       <c r="C2" s="4" t="s">
-        <v>216</v>
+        <v>210</v>
       </c>
       <c r="D2" s="4"/>
     </row>
     <row r="3" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="4" t="s">
-        <v>454</v>
+        <v>448</v>
       </c>
       <c r="B3" s="4" t="s">
-        <v>226</v>
+        <v>220</v>
       </c>
       <c r="C3" s="4" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="D3" s="4" t="s">
         <v>14</v>
@@ -4064,16 +4046,16 @@
     </row>
     <row r="4" customFormat="false" ht="72.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="7" t="s">
-        <v>455</v>
+        <v>449</v>
       </c>
       <c r="B4" s="7" t="s">
-        <v>456</v>
+        <v>450</v>
       </c>
       <c r="C4" s="7" t="s">
-        <v>457</v>
+        <v>451</v>
       </c>
       <c r="D4" s="7" t="s">
-        <v>458</v>
+        <v>452</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4283,1247 +4265,1247 @@
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="0" t="s">
-        <v>459</v>
+        <v>453</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="0" t="s">
-        <v>460</v>
+        <v>454</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="0" t="s">
-        <v>461</v>
+        <v>455</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="0" t="s">
-        <v>462</v>
+        <v>456</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="0" t="s">
-        <v>463</v>
+        <v>457</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="0" t="s">
-        <v>464</v>
+        <v>458</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="0" t="s">
-        <v>465</v>
+        <v>459</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="0" t="s">
-        <v>466</v>
+        <v>460</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="0" t="s">
-        <v>467</v>
+        <v>461</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="0" t="s">
-        <v>468</v>
+        <v>462</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="0" t="s">
-        <v>469</v>
+        <v>463</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="0" t="s">
-        <v>470</v>
+        <v>464</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="0" t="s">
-        <v>471</v>
+        <v>465</v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="0" t="s">
-        <v>472</v>
+        <v>466</v>
       </c>
     </row>
     <row r="15" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A15" s="0" t="s">
-        <v>473</v>
+        <v>467</v>
       </c>
     </row>
     <row r="16" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A16" s="0" t="s">
-        <v>474</v>
+        <v>468</v>
       </c>
     </row>
     <row r="17" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A17" s="0" t="s">
-        <v>475</v>
+        <v>469</v>
       </c>
     </row>
     <row r="18" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A18" s="0" t="s">
-        <v>476</v>
+        <v>470</v>
       </c>
     </row>
     <row r="19" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A19" s="0" t="s">
-        <v>477</v>
+        <v>471</v>
       </c>
     </row>
     <row r="20" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A20" s="0" t="s">
-        <v>478</v>
+        <v>472</v>
       </c>
     </row>
     <row r="21" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A21" s="0" t="s">
-        <v>479</v>
+        <v>473</v>
       </c>
     </row>
     <row r="22" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A22" s="0" t="s">
-        <v>480</v>
+        <v>474</v>
       </c>
     </row>
     <row r="23" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A23" s="0" t="s">
-        <v>481</v>
+        <v>475</v>
       </c>
     </row>
     <row r="24" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A24" s="0" t="s">
-        <v>482</v>
+        <v>476</v>
       </c>
     </row>
     <row r="25" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A25" s="0" t="s">
-        <v>483</v>
+        <v>477</v>
       </c>
     </row>
     <row r="26" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A26" s="0" t="s">
-        <v>484</v>
+        <v>478</v>
       </c>
     </row>
     <row r="27" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A27" s="0" t="s">
-        <v>485</v>
+        <v>479</v>
       </c>
     </row>
     <row r="28" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A28" s="0" t="s">
-        <v>486</v>
+        <v>480</v>
       </c>
     </row>
     <row r="29" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A29" s="0" t="s">
-        <v>487</v>
+        <v>481</v>
       </c>
     </row>
     <row r="30" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A30" s="0" t="s">
-        <v>488</v>
+        <v>482</v>
       </c>
     </row>
     <row r="31" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A31" s="0" t="s">
-        <v>489</v>
+        <v>483</v>
       </c>
     </row>
     <row r="32" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A32" s="0" t="s">
-        <v>490</v>
+        <v>484</v>
       </c>
     </row>
     <row r="33" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A33" s="0" t="s">
-        <v>491</v>
+        <v>485</v>
       </c>
     </row>
     <row r="34" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A34" s="0" t="s">
-        <v>492</v>
+        <v>486</v>
       </c>
     </row>
     <row r="35" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A35" s="0" t="s">
-        <v>493</v>
+        <v>487</v>
       </c>
     </row>
     <row r="36" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A36" s="0" t="s">
-        <v>494</v>
+        <v>488</v>
       </c>
     </row>
     <row r="37" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A37" s="0" t="s">
-        <v>495</v>
+        <v>489</v>
       </c>
     </row>
     <row r="38" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A38" s="0" t="s">
-        <v>496</v>
+        <v>490</v>
       </c>
     </row>
     <row r="39" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A39" s="0" t="s">
-        <v>497</v>
+        <v>491</v>
       </c>
     </row>
     <row r="40" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A40" s="0" t="s">
-        <v>498</v>
+        <v>492</v>
       </c>
     </row>
     <row r="41" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A41" s="0" t="s">
-        <v>499</v>
+        <v>493</v>
       </c>
     </row>
     <row r="42" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A42" s="0" t="s">
-        <v>500</v>
+        <v>494</v>
       </c>
     </row>
     <row r="43" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A43" s="0" t="s">
-        <v>501</v>
+        <v>495</v>
       </c>
     </row>
     <row r="44" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A44" s="0" t="s">
-        <v>502</v>
+        <v>496</v>
       </c>
     </row>
     <row r="45" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A45" s="0" t="s">
-        <v>503</v>
+        <v>497</v>
       </c>
     </row>
     <row r="46" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A46" s="0" t="s">
-        <v>504</v>
+        <v>498</v>
       </c>
     </row>
     <row r="47" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A47" s="0" t="s">
-        <v>505</v>
+        <v>499</v>
       </c>
     </row>
     <row r="48" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A48" s="0" t="s">
-        <v>506</v>
+        <v>500</v>
       </c>
     </row>
     <row r="49" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A49" s="0" t="s">
-        <v>507</v>
+        <v>501</v>
       </c>
     </row>
     <row r="50" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A50" s="0" t="s">
-        <v>508</v>
+        <v>502</v>
       </c>
     </row>
     <row r="51" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A51" s="0" t="s">
-        <v>509</v>
+        <v>503</v>
       </c>
     </row>
     <row r="52" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A52" s="0" t="s">
-        <v>510</v>
+        <v>504</v>
       </c>
     </row>
     <row r="53" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A53" s="0" t="s">
-        <v>511</v>
+        <v>505</v>
       </c>
     </row>
     <row r="54" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A54" s="0" t="s">
-        <v>512</v>
+        <v>506</v>
       </c>
     </row>
     <row r="55" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A55" s="0" t="s">
-        <v>513</v>
+        <v>507</v>
       </c>
     </row>
     <row r="56" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A56" s="0" t="s">
-        <v>514</v>
+        <v>508</v>
       </c>
     </row>
     <row r="57" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A57" s="0" t="s">
-        <v>515</v>
+        <v>509</v>
       </c>
     </row>
     <row r="58" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A58" s="0" t="s">
-        <v>516</v>
+        <v>510</v>
       </c>
     </row>
     <row r="59" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A59" s="0" t="s">
-        <v>517</v>
+        <v>511</v>
       </c>
     </row>
     <row r="60" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A60" s="0" t="s">
-        <v>518</v>
+        <v>512</v>
       </c>
     </row>
     <row r="61" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A61" s="0" t="s">
-        <v>519</v>
+        <v>513</v>
       </c>
     </row>
     <row r="62" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A62" s="0" t="s">
-        <v>520</v>
+        <v>514</v>
       </c>
     </row>
     <row r="63" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A63" s="0" t="s">
-        <v>521</v>
+        <v>515</v>
       </c>
     </row>
     <row r="64" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A64" s="0" t="s">
-        <v>522</v>
+        <v>516</v>
       </c>
     </row>
     <row r="65" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A65" s="0" t="s">
-        <v>523</v>
+        <v>517</v>
       </c>
     </row>
     <row r="66" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A66" s="0" t="s">
-        <v>524</v>
+        <v>518</v>
       </c>
     </row>
     <row r="67" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A67" s="0" t="s">
-        <v>525</v>
+        <v>519</v>
       </c>
     </row>
     <row r="68" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A68" s="0" t="s">
-        <v>526</v>
+        <v>520</v>
       </c>
     </row>
     <row r="69" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A69" s="0" t="s">
-        <v>527</v>
+        <v>521</v>
       </c>
     </row>
     <row r="70" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A70" s="0" t="s">
-        <v>528</v>
+        <v>522</v>
       </c>
     </row>
     <row r="71" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A71" s="0" t="s">
-        <v>529</v>
+        <v>523</v>
       </c>
     </row>
     <row r="72" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A72" s="0" t="s">
-        <v>530</v>
+        <v>524</v>
       </c>
     </row>
     <row r="73" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A73" s="0" t="s">
-        <v>531</v>
+        <v>525</v>
       </c>
     </row>
     <row r="74" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A74" s="0" t="s">
-        <v>532</v>
+        <v>526</v>
       </c>
     </row>
     <row r="75" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A75" s="0" t="s">
-        <v>533</v>
+        <v>527</v>
       </c>
     </row>
     <row r="76" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A76" s="0" t="s">
-        <v>534</v>
+        <v>528</v>
       </c>
     </row>
     <row r="77" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A77" s="0" t="s">
-        <v>535</v>
+        <v>529</v>
       </c>
     </row>
     <row r="78" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A78" s="0" t="s">
-        <v>536</v>
+        <v>530</v>
       </c>
     </row>
     <row r="79" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A79" s="0" t="s">
-        <v>537</v>
+        <v>531</v>
       </c>
     </row>
     <row r="80" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A80" s="0" t="s">
-        <v>538</v>
+        <v>532</v>
       </c>
     </row>
     <row r="81" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A81" s="0" t="s">
-        <v>539</v>
+        <v>533</v>
       </c>
     </row>
     <row r="82" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A82" s="0" t="s">
-        <v>540</v>
+        <v>534</v>
       </c>
     </row>
     <row r="83" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A83" s="0" t="s">
-        <v>541</v>
+        <v>535</v>
       </c>
     </row>
     <row r="84" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A84" s="0" t="s">
-        <v>542</v>
+        <v>536</v>
       </c>
     </row>
     <row r="85" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A85" s="0" t="s">
-        <v>543</v>
+        <v>537</v>
       </c>
     </row>
     <row r="86" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A86" s="0" t="s">
-        <v>544</v>
+        <v>538</v>
       </c>
     </row>
     <row r="87" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A87" s="0" t="s">
-        <v>545</v>
+        <v>539</v>
       </c>
     </row>
     <row r="88" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A88" s="0" t="s">
-        <v>546</v>
+        <v>540</v>
       </c>
     </row>
     <row r="89" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A89" s="0" t="s">
-        <v>547</v>
+        <v>541</v>
       </c>
     </row>
     <row r="90" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A90" s="0" t="s">
-        <v>548</v>
+        <v>542</v>
       </c>
     </row>
     <row r="91" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A91" s="0" t="s">
-        <v>549</v>
+        <v>543</v>
       </c>
     </row>
     <row r="92" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A92" s="0" t="s">
-        <v>550</v>
+        <v>544</v>
       </c>
     </row>
     <row r="93" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A93" s="0" t="s">
-        <v>551</v>
+        <v>545</v>
       </c>
     </row>
     <row r="94" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A94" s="0" t="s">
-        <v>552</v>
+        <v>546</v>
       </c>
     </row>
     <row r="95" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A95" s="0" t="s">
-        <v>553</v>
+        <v>547</v>
       </c>
     </row>
     <row r="96" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A96" s="0" t="s">
-        <v>554</v>
+        <v>548</v>
       </c>
     </row>
     <row r="97" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A97" s="0" t="s">
-        <v>555</v>
+        <v>549</v>
       </c>
     </row>
     <row r="98" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A98" s="0" t="s">
-        <v>556</v>
+        <v>550</v>
       </c>
     </row>
     <row r="99" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A99" s="0" t="s">
-        <v>557</v>
+        <v>551</v>
       </c>
     </row>
     <row r="100" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A100" s="0" t="s">
-        <v>558</v>
+        <v>552</v>
       </c>
     </row>
     <row r="101" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A101" s="0" t="s">
-        <v>223</v>
+        <v>217</v>
       </c>
     </row>
     <row r="102" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A102" s="0" t="s">
-        <v>559</v>
+        <v>553</v>
       </c>
     </row>
     <row r="103" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A103" s="0" t="s">
-        <v>560</v>
+        <v>554</v>
       </c>
     </row>
     <row r="104" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A104" s="0" t="s">
-        <v>561</v>
+        <v>555</v>
       </c>
     </row>
     <row r="105" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A105" s="0" t="s">
-        <v>562</v>
+        <v>556</v>
       </c>
     </row>
     <row r="106" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A106" s="0" t="s">
-        <v>563</v>
+        <v>557</v>
       </c>
     </row>
     <row r="107" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A107" s="0" t="s">
-        <v>564</v>
+        <v>558</v>
       </c>
     </row>
     <row r="108" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A108" s="0" t="s">
-        <v>565</v>
+        <v>559</v>
       </c>
     </row>
     <row r="109" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A109" s="0" t="s">
-        <v>566</v>
+        <v>560</v>
       </c>
     </row>
     <row r="110" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A110" s="0" t="s">
-        <v>567</v>
+        <v>561</v>
       </c>
     </row>
     <row r="111" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A111" s="0" t="s">
-        <v>568</v>
+        <v>562</v>
       </c>
     </row>
     <row r="112" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A112" s="0" t="s">
-        <v>569</v>
+        <v>563</v>
       </c>
     </row>
     <row r="113" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A113" s="0" t="s">
-        <v>570</v>
+        <v>564</v>
       </c>
     </row>
     <row r="114" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A114" s="0" t="s">
-        <v>571</v>
+        <v>565</v>
       </c>
     </row>
     <row r="115" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A115" s="0" t="s">
-        <v>572</v>
+        <v>566</v>
       </c>
     </row>
     <row r="116" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A116" s="0" t="s">
-        <v>573</v>
+        <v>567</v>
       </c>
     </row>
     <row r="117" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A117" s="0" t="s">
-        <v>574</v>
+        <v>568</v>
       </c>
     </row>
     <row r="118" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A118" s="0" t="s">
-        <v>575</v>
+        <v>569</v>
       </c>
     </row>
     <row r="119" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A119" s="0" t="s">
-        <v>576</v>
+        <v>570</v>
       </c>
     </row>
     <row r="120" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A120" s="0" t="s">
-        <v>577</v>
+        <v>571</v>
       </c>
     </row>
     <row r="121" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A121" s="0" t="s">
-        <v>578</v>
+        <v>572</v>
       </c>
     </row>
     <row r="122" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A122" s="0" t="s">
-        <v>579</v>
+        <v>573</v>
       </c>
     </row>
     <row r="123" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A123" s="0" t="s">
-        <v>580</v>
+        <v>574</v>
       </c>
     </row>
     <row r="124" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A124" s="0" t="s">
-        <v>581</v>
+        <v>575</v>
       </c>
     </row>
     <row r="125" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A125" s="0" t="s">
-        <v>582</v>
+        <v>576</v>
       </c>
     </row>
     <row r="126" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A126" s="0" t="s">
-        <v>583</v>
+        <v>577</v>
       </c>
     </row>
     <row r="127" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A127" s="0" t="s">
-        <v>584</v>
+        <v>578</v>
       </c>
     </row>
     <row r="128" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A128" s="0" t="s">
-        <v>585</v>
+        <v>579</v>
       </c>
     </row>
     <row r="129" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A129" s="0" t="s">
-        <v>586</v>
+        <v>580</v>
       </c>
     </row>
     <row r="130" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A130" s="0" t="s">
-        <v>587</v>
+        <v>581</v>
       </c>
     </row>
     <row r="131" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A131" s="0" t="s">
-        <v>588</v>
+        <v>582</v>
       </c>
     </row>
     <row r="132" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A132" s="0" t="s">
-        <v>589</v>
+        <v>583</v>
       </c>
     </row>
     <row r="133" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A133" s="0" t="s">
-        <v>590</v>
+        <v>584</v>
       </c>
     </row>
     <row r="134" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A134" s="0" t="s">
-        <v>591</v>
+        <v>585</v>
       </c>
     </row>
     <row r="135" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A135" s="0" t="s">
-        <v>592</v>
+        <v>586</v>
       </c>
     </row>
     <row r="136" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A136" s="0" t="s">
-        <v>593</v>
+        <v>587</v>
       </c>
     </row>
     <row r="137" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A137" s="0" t="s">
-        <v>594</v>
+        <v>588</v>
       </c>
     </row>
     <row r="138" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A138" s="0" t="s">
-        <v>595</v>
+        <v>589</v>
       </c>
     </row>
     <row r="139" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A139" s="0" t="s">
-        <v>596</v>
+        <v>590</v>
       </c>
     </row>
     <row r="140" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A140" s="0" t="s">
-        <v>597</v>
+        <v>591</v>
       </c>
     </row>
     <row r="141" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A141" s="0" t="s">
-        <v>598</v>
+        <v>592</v>
       </c>
     </row>
     <row r="142" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A142" s="0" t="s">
-        <v>599</v>
+        <v>593</v>
       </c>
     </row>
     <row r="143" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A143" s="0" t="s">
-        <v>600</v>
+        <v>594</v>
       </c>
     </row>
     <row r="144" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A144" s="0" t="s">
-        <v>601</v>
+        <v>595</v>
       </c>
     </row>
     <row r="145" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A145" s="0" t="s">
-        <v>602</v>
+        <v>596</v>
       </c>
     </row>
     <row r="146" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A146" s="0" t="s">
-        <v>603</v>
+        <v>597</v>
       </c>
     </row>
     <row r="147" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A147" s="0" t="s">
-        <v>604</v>
+        <v>598</v>
       </c>
     </row>
     <row r="148" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A148" s="0" t="s">
-        <v>605</v>
+        <v>599</v>
       </c>
     </row>
     <row r="149" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A149" s="0" t="s">
-        <v>606</v>
+        <v>600</v>
       </c>
     </row>
     <row r="150" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A150" s="0" t="s">
-        <v>607</v>
+        <v>601</v>
       </c>
     </row>
     <row r="151" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A151" s="0" t="s">
-        <v>608</v>
+        <v>602</v>
       </c>
     </row>
     <row r="152" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A152" s="0" t="s">
-        <v>609</v>
+        <v>603</v>
       </c>
     </row>
     <row r="153" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A153" s="0" t="s">
-        <v>610</v>
+        <v>604</v>
       </c>
     </row>
     <row r="154" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A154" s="0" t="s">
-        <v>611</v>
+        <v>605</v>
       </c>
     </row>
     <row r="155" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A155" s="0" t="s">
-        <v>612</v>
+        <v>606</v>
       </c>
     </row>
     <row r="156" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A156" s="0" t="s">
-        <v>613</v>
+        <v>607</v>
       </c>
     </row>
     <row r="157" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A157" s="0" t="s">
-        <v>614</v>
+        <v>608</v>
       </c>
     </row>
     <row r="158" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A158" s="0" t="s">
-        <v>615</v>
+        <v>609</v>
       </c>
     </row>
     <row r="159" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A159" s="0" t="s">
-        <v>616</v>
+        <v>610</v>
       </c>
     </row>
     <row r="160" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A160" s="0" t="s">
-        <v>617</v>
+        <v>611</v>
       </c>
     </row>
     <row r="161" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A161" s="0" t="s">
-        <v>618</v>
+        <v>612</v>
       </c>
     </row>
     <row r="162" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A162" s="0" t="s">
-        <v>619</v>
+        <v>613</v>
       </c>
     </row>
     <row r="163" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A163" s="0" t="s">
-        <v>620</v>
+        <v>614</v>
       </c>
     </row>
     <row r="164" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A164" s="0" t="s">
-        <v>621</v>
+        <v>615</v>
       </c>
     </row>
     <row r="165" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A165" s="0" t="s">
-        <v>622</v>
+        <v>616</v>
       </c>
     </row>
     <row r="166" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A166" s="0" t="s">
-        <v>623</v>
+        <v>617</v>
       </c>
     </row>
     <row r="167" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A167" s="0" t="s">
-        <v>624</v>
+        <v>618</v>
       </c>
     </row>
     <row r="168" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A168" s="0" t="s">
-        <v>625</v>
+        <v>619</v>
       </c>
     </row>
     <row r="169" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A169" s="0" t="s">
-        <v>626</v>
+        <v>620</v>
       </c>
     </row>
     <row r="170" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A170" s="0" t="s">
-        <v>627</v>
+        <v>621</v>
       </c>
     </row>
     <row r="171" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A171" s="0" t="s">
-        <v>628</v>
+        <v>622</v>
       </c>
     </row>
     <row r="172" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A172" s="0" t="s">
-        <v>629</v>
+        <v>623</v>
       </c>
     </row>
     <row r="173" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A173" s="0" t="s">
-        <v>630</v>
+        <v>624</v>
       </c>
     </row>
     <row r="174" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A174" s="0" t="s">
-        <v>631</v>
+        <v>625</v>
       </c>
     </row>
     <row r="175" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A175" s="0" t="s">
-        <v>632</v>
+        <v>626</v>
       </c>
     </row>
     <row r="176" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A176" s="0" t="s">
-        <v>633</v>
+        <v>627</v>
       </c>
     </row>
     <row r="177" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A177" s="0" t="s">
-        <v>634</v>
+        <v>628</v>
       </c>
     </row>
     <row r="178" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A178" s="0" t="s">
-        <v>635</v>
+        <v>629</v>
       </c>
     </row>
     <row r="179" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A179" s="0" t="s">
-        <v>636</v>
+        <v>630</v>
       </c>
     </row>
     <row r="180" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A180" s="0" t="s">
-        <v>637</v>
+        <v>631</v>
       </c>
     </row>
     <row r="181" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A181" s="0" t="s">
-        <v>638</v>
+        <v>632</v>
       </c>
     </row>
     <row r="182" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A182" s="0" t="s">
-        <v>639</v>
+        <v>633</v>
       </c>
     </row>
     <row r="183" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A183" s="0" t="s">
-        <v>640</v>
+        <v>634</v>
       </c>
     </row>
     <row r="184" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A184" s="0" t="s">
-        <v>641</v>
+        <v>635</v>
       </c>
     </row>
     <row r="185" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A185" s="0" t="s">
-        <v>642</v>
+        <v>636</v>
       </c>
     </row>
     <row r="186" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A186" s="0" t="s">
-        <v>643</v>
+        <v>637</v>
       </c>
     </row>
     <row r="187" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A187" s="0" t="s">
-        <v>644</v>
+        <v>638</v>
       </c>
     </row>
     <row r="188" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A188" s="0" t="s">
-        <v>645</v>
+        <v>639</v>
       </c>
     </row>
     <row r="189" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A189" s="0" t="s">
-        <v>646</v>
+        <v>640</v>
       </c>
     </row>
     <row r="190" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A190" s="0" t="s">
-        <v>647</v>
+        <v>641</v>
       </c>
     </row>
     <row r="191" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A191" s="0" t="s">
-        <v>648</v>
+        <v>642</v>
       </c>
     </row>
     <row r="192" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A192" s="0" t="s">
-        <v>649</v>
+        <v>643</v>
       </c>
     </row>
     <row r="193" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A193" s="0" t="s">
-        <v>650</v>
+        <v>644</v>
       </c>
     </row>
     <row r="194" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A194" s="0" t="s">
-        <v>651</v>
+        <v>645</v>
       </c>
     </row>
     <row r="195" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A195" s="0" t="s">
-        <v>652</v>
+        <v>646</v>
       </c>
     </row>
     <row r="196" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A196" s="0" t="s">
-        <v>653</v>
+        <v>647</v>
       </c>
     </row>
     <row r="197" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A197" s="0" t="s">
-        <v>654</v>
+        <v>648</v>
       </c>
     </row>
     <row r="198" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A198" s="0" t="s">
-        <v>655</v>
+        <v>649</v>
       </c>
     </row>
     <row r="199" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A199" s="0" t="s">
-        <v>656</v>
+        <v>650</v>
       </c>
     </row>
     <row r="200" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A200" s="0" t="s">
-        <v>657</v>
+        <v>651</v>
       </c>
     </row>
     <row r="201" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A201" s="0" t="s">
-        <v>658</v>
+        <v>652</v>
       </c>
     </row>
     <row r="202" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A202" s="0" t="s">
-        <v>659</v>
+        <v>653</v>
       </c>
     </row>
     <row r="203" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A203" s="0" t="s">
-        <v>660</v>
+        <v>654</v>
       </c>
     </row>
     <row r="204" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A204" s="0" t="s">
-        <v>661</v>
+        <v>655</v>
       </c>
     </row>
     <row r="205" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A205" s="0" t="s">
-        <v>662</v>
+        <v>656</v>
       </c>
     </row>
     <row r="206" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A206" s="0" t="s">
-        <v>663</v>
+        <v>657</v>
       </c>
     </row>
     <row r="207" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A207" s="0" t="s">
-        <v>664</v>
+        <v>658</v>
       </c>
     </row>
     <row r="208" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A208" s="0" t="s">
-        <v>665</v>
+        <v>659</v>
       </c>
     </row>
     <row r="209" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A209" s="0" t="s">
-        <v>666</v>
+        <v>660</v>
       </c>
     </row>
     <row r="210" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A210" s="0" t="s">
-        <v>667</v>
+        <v>661</v>
       </c>
     </row>
     <row r="211" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A211" s="0" t="s">
-        <v>668</v>
+        <v>662</v>
       </c>
     </row>
     <row r="212" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A212" s="0" t="s">
-        <v>669</v>
+        <v>663</v>
       </c>
     </row>
     <row r="213" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A213" s="0" t="s">
-        <v>670</v>
+        <v>664</v>
       </c>
     </row>
     <row r="214" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A214" s="0" t="s">
-        <v>671</v>
+        <v>665</v>
       </c>
     </row>
     <row r="215" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A215" s="0" t="s">
-        <v>672</v>
+        <v>666</v>
       </c>
     </row>
     <row r="216" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A216" s="0" t="s">
-        <v>673</v>
+        <v>667</v>
       </c>
     </row>
     <row r="217" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A217" s="0" t="s">
-        <v>674</v>
+        <v>668</v>
       </c>
     </row>
     <row r="218" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A218" s="0" t="s">
-        <v>675</v>
+        <v>669</v>
       </c>
     </row>
     <row r="219" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A219" s="0" t="s">
-        <v>676</v>
+        <v>670</v>
       </c>
     </row>
     <row r="220" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A220" s="0" t="s">
-        <v>677</v>
+        <v>671</v>
       </c>
     </row>
     <row r="221" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A221" s="0" t="s">
-        <v>678</v>
+        <v>672</v>
       </c>
     </row>
     <row r="222" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A222" s="0" t="s">
-        <v>679</v>
+        <v>673</v>
       </c>
     </row>
     <row r="223" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A223" s="0" t="s">
-        <v>680</v>
+        <v>674</v>
       </c>
     </row>
     <row r="224" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A224" s="0" t="s">
-        <v>681</v>
+        <v>675</v>
       </c>
     </row>
     <row r="225" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A225" s="0" t="s">
-        <v>682</v>
+        <v>676</v>
       </c>
     </row>
     <row r="226" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A226" s="0" t="s">
-        <v>683</v>
+        <v>677</v>
       </c>
     </row>
     <row r="227" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A227" s="0" t="s">
-        <v>684</v>
+        <v>678</v>
       </c>
     </row>
     <row r="228" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A228" s="0" t="s">
-        <v>685</v>
+        <v>679</v>
       </c>
     </row>
     <row r="229" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A229" s="0" t="s">
-        <v>686</v>
+        <v>680</v>
       </c>
     </row>
     <row r="230" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A230" s="0" t="s">
-        <v>687</v>
+        <v>681</v>
       </c>
     </row>
     <row r="231" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A231" s="0" t="s">
-        <v>688</v>
+        <v>682</v>
       </c>
     </row>
     <row r="232" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A232" s="0" t="s">
-        <v>689</v>
+        <v>683</v>
       </c>
     </row>
     <row r="233" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A233" s="0" t="s">
-        <v>690</v>
+        <v>684</v>
       </c>
     </row>
     <row r="234" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A234" s="0" t="s">
-        <v>691</v>
+        <v>685</v>
       </c>
     </row>
     <row r="235" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A235" s="0" t="s">
-        <v>692</v>
+        <v>686</v>
       </c>
     </row>
     <row r="236" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A236" s="0" t="s">
-        <v>693</v>
+        <v>687</v>
       </c>
     </row>
     <row r="237" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A237" s="0" t="s">
-        <v>694</v>
+        <v>688</v>
       </c>
     </row>
     <row r="238" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A238" s="0" t="s">
-        <v>695</v>
+        <v>689</v>
       </c>
     </row>
     <row r="239" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A239" s="0" t="s">
-        <v>696</v>
+        <v>690</v>
       </c>
     </row>
     <row r="240" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A240" s="0" t="s">
-        <v>697</v>
+        <v>691</v>
       </c>
     </row>
     <row r="241" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A241" s="0" t="s">
-        <v>698</v>
+        <v>692</v>
       </c>
     </row>
     <row r="242" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A242" s="0" t="s">
-        <v>699</v>
+        <v>693</v>
       </c>
     </row>
     <row r="243" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A243" s="0" t="s">
-        <v>700</v>
+        <v>694</v>
       </c>
     </row>
     <row r="244" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A244" s="0" t="s">
-        <v>701</v>
+        <v>695</v>
       </c>
     </row>
     <row r="245" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A245" s="0" t="s">
-        <v>702</v>
+        <v>696</v>
       </c>
     </row>
     <row r="246" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A246" s="0" t="s">
-        <v>703</v>
+        <v>697</v>
       </c>
     </row>
     <row r="247" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A247" s="0" t="s">
-        <v>704</v>
+        <v>698</v>
       </c>
     </row>
     <row r="248" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A248" s="0" t="s">
-        <v>705</v>
+        <v>699</v>
       </c>
     </row>
     <row r="249" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A249" s="0" t="s">
-        <v>706</v>
+        <v>700</v>
       </c>
     </row>
   </sheetData>
@@ -5544,7 +5526,7 @@
   </sheetPr>
   <dimension ref="A2:G136"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
@@ -5607,7 +5589,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="9" customFormat="false" ht="29.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="9" customFormat="false" ht="30" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="4" t="s">
         <v>8</v>
       </c>
@@ -5619,7 +5601,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="10" customFormat="false" ht="29.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="10" customFormat="false" ht="30" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="4" t="s">
         <v>17</v>
       </c>
@@ -5652,45 +5634,42 @@
       <c r="D13" s="7" t="s">
         <v>22</v>
       </c>
-      <c r="E13" s="0" t="s">
+    </row>
+    <row r="14" customFormat="false" ht="44.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A14" s="4" t="s">
         <v>23</v>
-      </c>
-    </row>
-    <row r="14" customFormat="false" ht="44" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A14" s="4" t="s">
-        <v>24</v>
       </c>
       <c r="B14" s="6"/>
       <c r="C14" s="7" t="s">
+        <v>24</v>
+      </c>
+      <c r="D14" s="7" t="s">
         <v>25</v>
-      </c>
-      <c r="D14" s="7" t="s">
-        <v>26</v>
       </c>
     </row>
     <row r="15" customFormat="false" ht="29.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A15" s="4" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="B15" s="4"/>
       <c r="C15" s="7" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="D15" s="7"/>
     </row>
     <row r="16" customFormat="false" ht="29.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A16" s="4" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="B16" s="4"/>
       <c r="C16" s="7" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="D16" s="7"/>
     </row>
     <row r="18" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A18" s="4" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="B18" s="4"/>
       <c r="C18" s="4" t="s">
@@ -5704,43 +5683,38 @@
       <c r="A19" s="6"/>
       <c r="B19" s="6"/>
       <c r="C19" s="7" t="s">
+        <v>31</v>
+      </c>
+      <c r="D19" s="7" t="s">
         <v>32</v>
       </c>
-      <c r="D19" s="7" t="s">
-        <v>33</v>
-      </c>
-      <c r="E19" s="0" t="s">
-        <v>34</v>
-      </c>
-      <c r="G19" s="8" t="s">
-        <v>35</v>
-      </c>
+      <c r="G19" s="8"/>
     </row>
     <row r="20" customFormat="false" ht="48.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A20" s="4" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="B20" s="4"/>
       <c r="C20" s="7" t="s">
-        <v>36</v>
+        <v>33</v>
       </c>
       <c r="D20" s="7"/>
       <c r="G20" s="8"/>
     </row>
     <row r="21" customFormat="false" ht="20.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A21" s="4" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="B21" s="4"/>
       <c r="C21" s="7" t="s">
-        <v>37</v>
+        <v>34</v>
       </c>
       <c r="D21" s="7"/>
     </row>
     <row r="22" customFormat="false" ht="20.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
     <row r="23" customFormat="false" ht="20.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A23" s="4" t="s">
-        <v>38</v>
+        <v>35</v>
       </c>
       <c r="B23" s="4"/>
       <c r="C23" s="4" t="s">
@@ -5753,103 +5727,85 @@
     <row r="24" customFormat="false" ht="20.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A24" s="4"/>
       <c r="B24" s="4" t="s">
-        <v>39</v>
+        <v>36</v>
       </c>
       <c r="C24" s="7" t="s">
-        <v>40</v>
+        <v>37</v>
       </c>
       <c r="D24" s="7" t="s">
-        <v>41</v>
-      </c>
-      <c r="E24" s="0" t="s">
-        <v>42</v>
+        <v>38</v>
       </c>
     </row>
     <row r="25" customFormat="false" ht="20.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A25" s="4"/>
       <c r="B25" s="4" t="s">
-        <v>43</v>
+        <v>39</v>
       </c>
       <c r="C25" s="7" t="s">
-        <v>44</v>
+        <v>40</v>
       </c>
       <c r="D25" s="7" t="s">
-        <v>41</v>
-      </c>
-      <c r="E25" s="0" t="s">
-        <v>42</v>
+        <v>38</v>
       </c>
     </row>
     <row r="26" customFormat="false" ht="20.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A26" s="4"/>
       <c r="B26" s="4" t="s">
-        <v>45</v>
+        <v>41</v>
       </c>
       <c r="C26" s="7" t="s">
-        <v>46</v>
+        <v>42</v>
       </c>
       <c r="D26" s="7" t="s">
-        <v>41</v>
-      </c>
-      <c r="E26" s="0" t="s">
-        <v>42</v>
+        <v>38</v>
       </c>
     </row>
     <row r="27" customFormat="false" ht="20.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A27" s="4"/>
       <c r="B27" s="4" t="s">
-        <v>47</v>
+        <v>43</v>
       </c>
       <c r="C27" s="7" t="s">
-        <v>48</v>
+        <v>44</v>
       </c>
       <c r="D27" s="7" t="s">
-        <v>41</v>
-      </c>
-      <c r="E27" s="0" t="s">
-        <v>42</v>
+        <v>38</v>
       </c>
     </row>
     <row r="28" customFormat="false" ht="20.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A28" s="4"/>
       <c r="B28" s="4" t="s">
-        <v>49</v>
+        <v>45</v>
       </c>
       <c r="C28" s="7" t="s">
-        <v>50</v>
+        <v>46</v>
       </c>
       <c r="D28" s="7" t="s">
-        <v>41</v>
-      </c>
-      <c r="E28" s="0" t="s">
-        <v>42</v>
+        <v>38</v>
       </c>
     </row>
     <row r="29" customFormat="false" ht="37.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A29" s="4"/>
       <c r="B29" s="9" t="s">
-        <v>51</v>
+        <v>47</v>
       </c>
       <c r="C29" s="7" t="s">
-        <v>52</v>
+        <v>48</v>
       </c>
       <c r="D29" s="7" t="s">
-        <v>41</v>
-      </c>
-      <c r="E29" s="0" t="s">
-        <v>42</v>
+        <v>38</v>
       </c>
     </row>
     <row r="30" customFormat="false" ht="20.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A30" s="4"/>
       <c r="B30" s="4" t="s">
-        <v>53</v>
+        <v>49</v>
       </c>
       <c r="C30" s="7" t="s">
-        <v>54</v>
+        <v>50</v>
       </c>
       <c r="D30" s="7" t="s">
-        <v>41</v>
+        <v>38</v>
       </c>
     </row>
     <row r="31" customFormat="false" ht="20.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -5859,26 +5815,26 @@
       </c>
       <c r="C31" s="7"/>
       <c r="D31" s="7" t="s">
-        <v>55</v>
+        <v>51</v>
       </c>
     </row>
     <row r="32" customFormat="false" ht="20.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A32" s="4" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="B32" s="4"/>
       <c r="C32" s="7" t="s">
-        <v>56</v>
+        <v>52</v>
       </c>
       <c r="D32" s="7"/>
     </row>
     <row r="33" customFormat="false" ht="20.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A33" s="4" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="B33" s="4"/>
       <c r="C33" s="7" t="s">
-        <v>57</v>
+        <v>53</v>
       </c>
       <c r="D33" s="7"/>
     </row>
@@ -5895,55 +5851,52 @@
     </row>
     <row r="36" customFormat="false" ht="74.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A36" s="9" t="s">
-        <v>58</v>
+        <v>54</v>
       </c>
       <c r="B36" s="4"/>
       <c r="C36" s="7" t="s">
-        <v>59</v>
+        <v>55</v>
       </c>
       <c r="D36" s="7" t="s">
-        <v>60</v>
-      </c>
-      <c r="E36" s="0" t="s">
-        <v>42</v>
+        <v>56</v>
       </c>
     </row>
     <row r="37" customFormat="false" ht="74.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A37" s="4" t="s">
-        <v>61</v>
+        <v>57</v>
       </c>
       <c r="B37" s="4"/>
       <c r="C37" s="7" t="s">
-        <v>62</v>
+        <v>58</v>
       </c>
       <c r="D37" s="7" t="s">
-        <v>63</v>
+        <v>59</v>
       </c>
     </row>
     <row r="38" customFormat="false" ht="20.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A38" s="4" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="B38" s="4"/>
       <c r="C38" s="7" t="s">
-        <v>64</v>
+        <v>60</v>
       </c>
       <c r="D38" s="7"/>
     </row>
     <row r="39" customFormat="false" ht="20.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A39" s="4" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="B39" s="4"/>
       <c r="C39" s="7" t="s">
-        <v>65</v>
+        <v>61</v>
       </c>
       <c r="D39" s="7"/>
     </row>
     <row r="40" customFormat="false" ht="20.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
     <row r="41" customFormat="false" ht="20.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A41" s="4" t="s">
-        <v>66</v>
+        <v>62</v>
       </c>
       <c r="B41" s="4"/>
       <c r="C41" s="4" t="s">
@@ -5955,80 +5908,74 @@
     </row>
     <row r="42" customFormat="false" ht="20.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A42" s="4" t="s">
-        <v>67</v>
+        <v>63</v>
       </c>
       <c r="B42" s="4"/>
       <c r="C42" s="7" t="s">
-        <v>68</v>
+        <v>64</v>
       </c>
       <c r="D42" s="7" t="s">
-        <v>69</v>
-      </c>
-      <c r="E42" s="0" t="s">
-        <v>70</v>
+        <v>65</v>
       </c>
       <c r="F42" s="3"/>
     </row>
     <row r="43" customFormat="false" ht="20.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A43" s="4" t="s">
-        <v>71</v>
+        <v>66</v>
       </c>
       <c r="B43" s="4"/>
       <c r="C43" s="7" t="s">
-        <v>72</v>
+        <v>67</v>
       </c>
       <c r="D43" s="7" t="s">
-        <v>73</v>
-      </c>
-      <c r="E43" s="0" t="s">
-        <v>74</v>
+        <v>68</v>
       </c>
       <c r="F43" s="3"/>
     </row>
     <row r="44" customFormat="false" ht="20.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A44" s="10" t="s">
-        <v>75</v>
+        <v>69</v>
       </c>
       <c r="B44" s="11"/>
       <c r="C44" s="7" t="s">
-        <v>76</v>
+        <v>70</v>
       </c>
       <c r="D44" s="7" t="s">
-        <v>77</v>
+        <v>71</v>
       </c>
       <c r="F44" s="3"/>
     </row>
     <row r="45" customFormat="false" ht="20.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A45" s="4" t="s">
-        <v>78</v>
+        <v>72</v>
       </c>
       <c r="B45" s="4"/>
       <c r="C45" s="7" t="s">
-        <v>79</v>
+        <v>73</v>
       </c>
       <c r="D45" s="7" t="s">
-        <v>80</v>
+        <v>74</v>
       </c>
       <c r="F45" s="3"/>
     </row>
     <row r="46" customFormat="false" ht="20.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A46" s="4" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="B46" s="4"/>
       <c r="C46" s="7" t="s">
-        <v>81</v>
+        <v>75</v>
       </c>
       <c r="D46" s="7"/>
       <c r="F46" s="3"/>
     </row>
     <row r="47" customFormat="false" ht="20.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A47" s="4" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="B47" s="4"/>
       <c r="C47" s="7" t="s">
-        <v>82</v>
+        <v>76</v>
       </c>
       <c r="D47" s="7"/>
       <c r="F47" s="3"/>
@@ -6038,7 +5985,7 @@
     </row>
     <row r="49" customFormat="false" ht="20.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A49" s="4" t="s">
-        <v>83</v>
+        <v>77</v>
       </c>
       <c r="B49" s="4"/>
       <c r="C49" s="4" t="s">
@@ -6052,29 +5999,29 @@
       <c r="A50" s="4"/>
       <c r="B50" s="4"/>
       <c r="C50" s="7" t="s">
-        <v>84</v>
+        <v>78</v>
       </c>
       <c r="D50" s="7" t="s">
-        <v>85</v>
+        <v>79</v>
       </c>
     </row>
     <row r="51" customFormat="false" ht="20.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A51" s="4" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="B51" s="4"/>
       <c r="C51" s="7" t="s">
-        <v>86</v>
+        <v>80</v>
       </c>
       <c r="D51" s="7"/>
     </row>
     <row r="52" customFormat="false" ht="20.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A52" s="4" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="B52" s="4"/>
       <c r="C52" s="7" t="s">
-        <v>87</v>
+        <v>81</v>
       </c>
       <c r="D52" s="7"/>
     </row>
@@ -6091,33 +6038,33 @@
     </row>
     <row r="55" customFormat="false" ht="20.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A55" s="10" t="s">
-        <v>88</v>
+        <v>82</v>
       </c>
       <c r="B55" s="11"/>
       <c r="C55" s="7" t="s">
-        <v>89</v>
+        <v>83</v>
       </c>
       <c r="D55" s="7" t="s">
-        <v>90</v>
+        <v>84</v>
       </c>
     </row>
     <row r="56" customFormat="false" ht="20.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A56" s="4" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="B56" s="11"/>
       <c r="C56" s="7" t="s">
-        <v>91</v>
+        <v>85</v>
       </c>
       <c r="D56" s="7"/>
     </row>
     <row r="57" customFormat="false" ht="20.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A57" s="4" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="B57" s="11"/>
       <c r="C57" s="7" t="s">
-        <v>92</v>
+        <v>86</v>
       </c>
       <c r="D57" s="7"/>
     </row>
@@ -6134,76 +6081,64 @@
     </row>
     <row r="60" customFormat="false" ht="20.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A60" s="4" t="s">
-        <v>93</v>
+        <v>87</v>
       </c>
       <c r="B60" s="4" t="s">
-        <v>94</v>
+        <v>88</v>
       </c>
       <c r="C60" s="7" t="s">
-        <v>95</v>
+        <v>89</v>
       </c>
       <c r="D60" s="7" t="s">
-        <v>41</v>
-      </c>
-      <c r="E60" s="0" t="s">
-        <v>42</v>
+        <v>38</v>
       </c>
     </row>
     <row r="61" customFormat="false" ht="20.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A61" s="4"/>
       <c r="B61" s="4" t="s">
-        <v>96</v>
+        <v>90</v>
       </c>
       <c r="C61" s="7" t="s">
-        <v>97</v>
+        <v>91</v>
       </c>
       <c r="D61" s="7" t="s">
-        <v>41</v>
-      </c>
-      <c r="E61" s="0" t="s">
-        <v>42</v>
+        <v>38</v>
       </c>
     </row>
     <row r="62" customFormat="false" ht="20.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A62" s="4"/>
       <c r="B62" s="4" t="s">
-        <v>98</v>
+        <v>92</v>
       </c>
       <c r="C62" s="7" t="s">
-        <v>99</v>
+        <v>93</v>
       </c>
       <c r="D62" s="7" t="s">
-        <v>41</v>
-      </c>
-      <c r="E62" s="0" t="s">
-        <v>42</v>
+        <v>38</v>
       </c>
     </row>
     <row r="63" customFormat="false" ht="20.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A63" s="4"/>
       <c r="B63" s="4" t="s">
-        <v>100</v>
+        <v>94</v>
       </c>
       <c r="C63" s="7" t="s">
-        <v>101</v>
+        <v>95</v>
       </c>
       <c r="D63" s="7" t="s">
-        <v>41</v>
-      </c>
-      <c r="E63" s="0" t="s">
-        <v>42</v>
+        <v>38</v>
       </c>
     </row>
     <row r="64" customFormat="false" ht="20.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A64" s="4"/>
       <c r="B64" s="4" t="s">
-        <v>53</v>
+        <v>49</v>
       </c>
       <c r="C64" s="7" t="s">
-        <v>102</v>
+        <v>96</v>
       </c>
       <c r="D64" s="7" t="s">
-        <v>41</v>
+        <v>38</v>
       </c>
     </row>
     <row r="65" customFormat="false" ht="20.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -6213,26 +6148,26 @@
       </c>
       <c r="C65" s="7"/>
       <c r="D65" s="7" t="s">
-        <v>103</v>
+        <v>97</v>
       </c>
     </row>
     <row r="66" customFormat="false" ht="20.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A66" s="4" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="B66" s="4"/>
       <c r="C66" s="7" t="s">
-        <v>104</v>
+        <v>98</v>
       </c>
       <c r="D66" s="7"/>
     </row>
     <row r="67" customFormat="false" ht="20.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A67" s="4" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="B67" s="4"/>
       <c r="C67" s="7" t="s">
-        <v>105</v>
+        <v>99</v>
       </c>
       <c r="D67" s="7"/>
     </row>
@@ -6249,61 +6184,52 @@
     </row>
     <row r="70" customFormat="false" ht="20.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A70" s="4" t="s">
-        <v>106</v>
+        <v>100</v>
       </c>
       <c r="B70" s="4" t="s">
-        <v>107</v>
+        <v>101</v>
       </c>
       <c r="C70" s="7" t="s">
-        <v>108</v>
+        <v>102</v>
       </c>
       <c r="D70" s="7" t="s">
-        <v>41</v>
-      </c>
-      <c r="E70" s="0" t="s">
-        <v>42</v>
+        <v>38</v>
       </c>
     </row>
     <row r="71" customFormat="false" ht="20.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A71" s="4"/>
       <c r="B71" s="4" t="s">
-        <v>109</v>
+        <v>103</v>
       </c>
       <c r="C71" s="7" t="s">
-        <v>110</v>
+        <v>104</v>
       </c>
       <c r="D71" s="7" t="s">
-        <v>41</v>
-      </c>
-      <c r="E71" s="0" t="s">
-        <v>42</v>
+        <v>38</v>
       </c>
     </row>
     <row r="72" customFormat="false" ht="20.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A72" s="4"/>
       <c r="B72" s="4" t="s">
-        <v>111</v>
+        <v>105</v>
       </c>
       <c r="C72" s="7" t="s">
-        <v>112</v>
+        <v>106</v>
       </c>
       <c r="D72" s="7" t="s">
-        <v>41</v>
-      </c>
-      <c r="E72" s="0" t="s">
-        <v>42</v>
+        <v>38</v>
       </c>
     </row>
     <row r="73" customFormat="false" ht="20.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A73" s="4"/>
       <c r="B73" s="4" t="s">
-        <v>53</v>
+        <v>49</v>
       </c>
       <c r="C73" s="7" t="s">
-        <v>113</v>
+        <v>107</v>
       </c>
       <c r="D73" s="7" t="s">
-        <v>41</v>
+        <v>38</v>
       </c>
     </row>
     <row r="74" customFormat="false" ht="20.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -6313,26 +6239,26 @@
       </c>
       <c r="C74" s="7"/>
       <c r="D74" s="7" t="s">
-        <v>114</v>
+        <v>108</v>
       </c>
     </row>
     <row r="75" customFormat="false" ht="20.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A75" s="4" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="B75" s="4"/>
       <c r="C75" s="7" t="s">
-        <v>115</v>
+        <v>109</v>
       </c>
       <c r="D75" s="7"/>
     </row>
     <row r="76" customFormat="false" ht="20.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A76" s="4" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="B76" s="4"/>
       <c r="C76" s="7" t="s">
-        <v>116</v>
+        <v>110</v>
       </c>
       <c r="D76" s="7"/>
     </row>
@@ -6349,36 +6275,33 @@
     </row>
     <row r="79" customFormat="false" ht="20.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A79" s="10" t="s">
-        <v>117</v>
+        <v>111</v>
       </c>
       <c r="B79" s="11"/>
       <c r="C79" s="7" t="s">
-        <v>118</v>
+        <v>112</v>
       </c>
       <c r="D79" s="7" t="s">
-        <v>119</v>
-      </c>
-      <c r="E79" s="0" t="s">
-        <v>42</v>
+        <v>113</v>
       </c>
     </row>
     <row r="80" customFormat="false" ht="20.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A80" s="4" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="B80" s="11"/>
       <c r="C80" s="7" t="s">
-        <v>120</v>
+        <v>114</v>
       </c>
       <c r="D80" s="7"/>
     </row>
     <row r="81" customFormat="false" ht="20.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A81" s="4" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="B81" s="11"/>
       <c r="C81" s="7" t="s">
-        <v>121</v>
+        <v>115</v>
       </c>
       <c r="D81" s="7"/>
     </row>
@@ -6395,48 +6318,45 @@
     </row>
     <row r="84" customFormat="false" ht="38.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A84" s="9" t="s">
-        <v>122</v>
+        <v>116</v>
       </c>
       <c r="B84" s="4"/>
       <c r="C84" s="7" t="s">
-        <v>123</v>
+        <v>117</v>
       </c>
       <c r="D84" s="7" t="s">
-        <v>124</v>
-      </c>
-      <c r="E84" s="0" t="s">
-        <v>42</v>
+        <v>118</v>
       </c>
     </row>
     <row r="85" customFormat="false" ht="20.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A85" s="4" t="s">
-        <v>61</v>
+        <v>57</v>
       </c>
       <c r="B85" s="4"/>
       <c r="C85" s="7" t="s">
-        <v>125</v>
+        <v>119</v>
       </c>
       <c r="D85" s="7" t="s">
-        <v>126</v>
+        <v>120</v>
       </c>
     </row>
     <row r="86" customFormat="false" ht="20.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A86" s="4" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="B86" s="4"/>
       <c r="C86" s="7" t="s">
-        <v>127</v>
+        <v>121</v>
       </c>
       <c r="D86" s="7"/>
     </row>
     <row r="87" customFormat="false" ht="20.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A87" s="4" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="B87" s="4"/>
       <c r="C87" s="7" t="s">
-        <v>128</v>
+        <v>122</v>
       </c>
       <c r="D87" s="7"/>
     </row>
@@ -6453,76 +6373,64 @@
     </row>
     <row r="90" customFormat="false" ht="20.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A90" s="4" t="s">
-        <v>129</v>
+        <v>123</v>
       </c>
       <c r="B90" s="4" t="s">
-        <v>130</v>
+        <v>124</v>
       </c>
       <c r="C90" s="7" t="s">
-        <v>131</v>
+        <v>125</v>
       </c>
       <c r="D90" s="7" t="s">
-        <v>41</v>
-      </c>
-      <c r="E90" s="0" t="s">
-        <v>42</v>
+        <v>38</v>
       </c>
     </row>
     <row r="91" customFormat="false" ht="20.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A91" s="4"/>
       <c r="B91" s="4" t="s">
-        <v>132</v>
+        <v>126</v>
       </c>
       <c r="C91" s="7" t="s">
-        <v>133</v>
+        <v>127</v>
       </c>
       <c r="D91" s="7" t="s">
-        <v>41</v>
-      </c>
-      <c r="E91" s="0" t="s">
-        <v>42</v>
+        <v>38</v>
       </c>
     </row>
     <row r="92" customFormat="false" ht="20.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A92" s="4"/>
       <c r="B92" s="4" t="s">
-        <v>134</v>
+        <v>128</v>
       </c>
       <c r="C92" s="7" t="s">
-        <v>135</v>
+        <v>129</v>
       </c>
       <c r="D92" s="7" t="s">
-        <v>41</v>
-      </c>
-      <c r="E92" s="0" t="s">
-        <v>42</v>
+        <v>38</v>
       </c>
     </row>
     <row r="93" customFormat="false" ht="20.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A93" s="4"/>
       <c r="B93" s="4" t="s">
-        <v>136</v>
+        <v>130</v>
       </c>
       <c r="C93" s="7" t="s">
-        <v>137</v>
+        <v>131</v>
       </c>
       <c r="D93" s="7" t="s">
-        <v>41</v>
-      </c>
-      <c r="E93" s="0" t="s">
-        <v>42</v>
+        <v>38</v>
       </c>
     </row>
     <row r="94" customFormat="false" ht="20.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A94" s="4"/>
       <c r="B94" s="4" t="s">
-        <v>53</v>
+        <v>49</v>
       </c>
       <c r="C94" s="7" t="s">
-        <v>138</v>
+        <v>132</v>
       </c>
       <c r="D94" s="7" t="s">
-        <v>41</v>
+        <v>38</v>
       </c>
     </row>
     <row r="95" customFormat="false" ht="20.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -6532,32 +6440,32 @@
       </c>
       <c r="C95" s="7"/>
       <c r="D95" s="7" t="s">
-        <v>139</v>
+        <v>133</v>
       </c>
     </row>
     <row r="96" customFormat="false" ht="20.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A96" s="4" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="B96" s="4"/>
       <c r="C96" s="7" t="s">
-        <v>140</v>
+        <v>134</v>
       </c>
       <c r="D96" s="7"/>
     </row>
     <row r="97" customFormat="false" ht="20.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A97" s="4" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="B97" s="4"/>
       <c r="C97" s="7" t="s">
-        <v>141</v>
+        <v>135</v>
       </c>
       <c r="D97" s="7"/>
     </row>
     <row r="99" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A99" s="4" t="s">
-        <v>142</v>
+        <v>136</v>
       </c>
       <c r="B99" s="4"/>
       <c r="C99" s="4" t="s">
@@ -6569,53 +6477,53 @@
     </row>
     <row r="100" customFormat="false" ht="58.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A100" s="4" t="s">
-        <v>143</v>
+        <v>137</v>
       </c>
       <c r="B100" s="4" t="s">
-        <v>144</v>
+        <v>138</v>
       </c>
       <c r="C100" s="7" t="s">
-        <v>145</v>
+        <v>139</v>
       </c>
       <c r="D100" s="7" t="s">
-        <v>146</v>
+        <v>140</v>
       </c>
     </row>
     <row r="101" customFormat="false" ht="58.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A101" s="4"/>
       <c r="B101" s="4" t="s">
-        <v>147</v>
+        <v>141</v>
       </c>
       <c r="C101" s="7" t="s">
-        <v>148</v>
+        <v>142</v>
       </c>
       <c r="D101" s="7" t="s">
-        <v>149</v>
+        <v>143</v>
       </c>
     </row>
     <row r="102" customFormat="false" ht="30" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A102" s="4" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="B102" s="4"/>
       <c r="C102" s="7" t="s">
-        <v>150</v>
+        <v>144</v>
       </c>
       <c r="D102" s="7"/>
     </row>
     <row r="103" customFormat="false" ht="29.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A103" s="4" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="B103" s="4"/>
       <c r="C103" s="7" t="s">
-        <v>151</v>
+        <v>145</v>
       </c>
       <c r="D103" s="7"/>
     </row>
     <row r="105" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A105" s="4" t="s">
-        <v>152</v>
+        <v>146</v>
       </c>
       <c r="B105" s="4"/>
       <c r="C105" s="4" t="s">
@@ -6627,191 +6535,161 @@
     </row>
     <row r="106" customFormat="false" ht="44" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A106" s="4" t="s">
-        <v>153</v>
+        <v>147</v>
       </c>
       <c r="B106" s="4"/>
       <c r="C106" s="7" t="s">
-        <v>154</v>
+        <v>148</v>
       </c>
       <c r="D106" s="7" t="s">
-        <v>155</v>
+        <v>149</v>
       </c>
     </row>
     <row r="107" customFormat="false" ht="44.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A107" s="4" t="s">
-        <v>156</v>
+        <v>150</v>
       </c>
       <c r="B107" s="4"/>
       <c r="C107" s="7" t="s">
-        <v>157</v>
+        <v>151</v>
       </c>
       <c r="D107" s="7" t="s">
-        <v>158</v>
+        <v>152</v>
       </c>
       <c r="E107" s="12"/>
     </row>
     <row r="108" customFormat="false" ht="58.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A108" s="4" t="s">
-        <v>159</v>
+        <v>153</v>
       </c>
       <c r="B108" s="4" t="s">
-        <v>160</v>
+        <v>154</v>
       </c>
       <c r="C108" s="7" t="s">
-        <v>161</v>
+        <v>155</v>
       </c>
       <c r="D108" s="7" t="s">
-        <v>41</v>
-      </c>
-      <c r="E108" s="0" t="s">
-        <v>42</v>
+        <v>38</v>
       </c>
     </row>
     <row r="109" customFormat="false" ht="44" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A109" s="4"/>
       <c r="B109" s="4" t="s">
-        <v>162</v>
+        <v>156</v>
       </c>
       <c r="C109" s="7" t="s">
-        <v>163</v>
+        <v>157</v>
       </c>
       <c r="D109" s="7" t="s">
-        <v>41</v>
-      </c>
-      <c r="E109" s="0" t="s">
-        <v>42</v>
+        <v>38</v>
       </c>
     </row>
     <row r="110" customFormat="false" ht="44" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A110" s="4"/>
       <c r="B110" s="4" t="s">
-        <v>164</v>
+        <v>158</v>
       </c>
       <c r="C110" s="7" t="s">
-        <v>165</v>
+        <v>159</v>
       </c>
       <c r="D110" s="7" t="s">
-        <v>41</v>
-      </c>
-      <c r="E110" s="0" t="s">
-        <v>42</v>
+        <v>38</v>
       </c>
     </row>
     <row r="111" customFormat="false" ht="44" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A111" s="4"/>
       <c r="B111" s="4" t="s">
-        <v>166</v>
+        <v>160</v>
       </c>
       <c r="C111" s="7" t="s">
-        <v>167</v>
+        <v>161</v>
       </c>
       <c r="D111" s="7" t="s">
-        <v>41</v>
-      </c>
-      <c r="E111" s="0" t="s">
-        <v>42</v>
+        <v>38</v>
       </c>
     </row>
     <row r="112" customFormat="false" ht="44" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A112" s="4"/>
       <c r="B112" s="4" t="s">
-        <v>168</v>
+        <v>162</v>
       </c>
       <c r="C112" s="7" t="s">
-        <v>169</v>
+        <v>163</v>
       </c>
       <c r="D112" s="7" t="s">
-        <v>41</v>
-      </c>
-      <c r="E112" s="0" t="s">
-        <v>42</v>
+        <v>38</v>
       </c>
     </row>
     <row r="113" customFormat="false" ht="44" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A113" s="4"/>
       <c r="B113" s="4" t="s">
-        <v>170</v>
+        <v>164</v>
       </c>
       <c r="C113" s="7" t="s">
-        <v>171</v>
+        <v>165</v>
       </c>
       <c r="D113" s="7" t="s">
-        <v>41</v>
-      </c>
-      <c r="E113" s="0" t="s">
-        <v>42</v>
+        <v>38</v>
       </c>
     </row>
     <row r="114" customFormat="false" ht="44" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A114" s="4"/>
       <c r="B114" s="4" t="s">
-        <v>172</v>
+        <v>166</v>
       </c>
       <c r="C114" s="7" t="s">
-        <v>173</v>
+        <v>167</v>
       </c>
       <c r="D114" s="7" t="s">
-        <v>41</v>
-      </c>
-      <c r="E114" s="0" t="s">
-        <v>42</v>
+        <v>38</v>
       </c>
     </row>
     <row r="115" customFormat="false" ht="44" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A115" s="4"/>
       <c r="B115" s="4" t="s">
-        <v>174</v>
+        <v>168</v>
       </c>
       <c r="C115" s="7" t="s">
-        <v>175</v>
+        <v>169</v>
       </c>
       <c r="D115" s="7" t="s">
-        <v>41</v>
-      </c>
-      <c r="E115" s="0" t="s">
-        <v>42</v>
+        <v>38</v>
       </c>
     </row>
     <row r="116" customFormat="false" ht="44" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A116" s="4"/>
       <c r="B116" s="4" t="s">
-        <v>176</v>
+        <v>170</v>
       </c>
       <c r="C116" s="7" t="s">
-        <v>177</v>
+        <v>171</v>
       </c>
       <c r="D116" s="7" t="s">
-        <v>41</v>
-      </c>
-      <c r="E116" s="0" t="s">
-        <v>42</v>
+        <v>38</v>
       </c>
     </row>
     <row r="117" customFormat="false" ht="44" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A117" s="4"/>
       <c r="B117" s="4" t="s">
-        <v>178</v>
+        <v>172</v>
       </c>
       <c r="C117" s="7" t="s">
-        <v>179</v>
+        <v>173</v>
       </c>
       <c r="D117" s="7" t="s">
-        <v>41</v>
-      </c>
-      <c r="E117" s="0" t="s">
-        <v>42</v>
+        <v>38</v>
       </c>
     </row>
     <row r="118" customFormat="false" ht="44" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A118" s="4"/>
       <c r="B118" s="4" t="s">
-        <v>53</v>
+        <v>49</v>
       </c>
       <c r="C118" s="7" t="s">
-        <v>180</v>
+        <v>174</v>
       </c>
       <c r="D118" s="7" t="s">
-        <v>41</v>
+        <v>38</v>
       </c>
       <c r="E118" s="12"/>
     </row>
@@ -6821,96 +6699,96 @@
         <v>14</v>
       </c>
       <c r="C119" s="7" t="s">
-        <v>41</v>
+        <v>38</v>
       </c>
       <c r="D119" s="7" t="s">
-        <v>181</v>
+        <v>175</v>
       </c>
       <c r="E119" s="12"/>
     </row>
     <row r="120" customFormat="false" ht="44" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A120" s="4" t="s">
-        <v>182</v>
+        <v>176</v>
       </c>
       <c r="B120" s="4"/>
       <c r="C120" s="7" t="s">
-        <v>183</v>
+        <v>177</v>
       </c>
       <c r="D120" s="7" t="s">
-        <v>184</v>
+        <v>178</v>
       </c>
       <c r="E120" s="13" t="s">
-        <v>185</v>
+        <v>179</v>
       </c>
     </row>
     <row r="121" customFormat="false" ht="44" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A121" s="4" t="s">
-        <v>186</v>
+        <v>180</v>
       </c>
       <c r="B121" s="4"/>
       <c r="C121" s="7" t="s">
-        <v>187</v>
+        <v>181</v>
       </c>
       <c r="D121" s="7" t="s">
-        <v>188</v>
+        <v>182</v>
       </c>
       <c r="E121" s="0" t="s">
-        <v>189</v>
+        <v>183</v>
       </c>
     </row>
     <row r="122" customFormat="false" ht="44" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A122" s="4" t="s">
-        <v>190</v>
+        <v>184</v>
       </c>
       <c r="B122" s="4"/>
       <c r="C122" s="7" t="s">
-        <v>191</v>
+        <v>185</v>
       </c>
       <c r="D122" s="7" t="s">
-        <v>192</v>
+        <v>186</v>
       </c>
       <c r="E122" s="13" t="s">
-        <v>193</v>
+        <v>187</v>
       </c>
     </row>
     <row r="123" customFormat="false" ht="44" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A123" s="4" t="s">
-        <v>194</v>
+        <v>188</v>
       </c>
       <c r="B123" s="4"/>
       <c r="C123" s="7" t="s">
-        <v>195</v>
+        <v>189</v>
       </c>
       <c r="D123" s="7" t="s">
-        <v>196</v>
+        <v>190</v>
       </c>
       <c r="E123" s="3" t="s">
-        <v>189</v>
+        <v>183</v>
       </c>
     </row>
     <row r="124" customFormat="false" ht="29.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A124" s="4" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="B124" s="4"/>
       <c r="C124" s="7" t="s">
-        <v>197</v>
+        <v>191</v>
       </c>
       <c r="D124" s="7"/>
     </row>
     <row r="125" customFormat="false" ht="29.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A125" s="4" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="B125" s="4"/>
       <c r="C125" s="7" t="s">
-        <v>198</v>
+        <v>192</v>
       </c>
       <c r="D125" s="7"/>
     </row>
     <row r="127" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A127" s="4" t="s">
-        <v>199</v>
+        <v>193</v>
       </c>
       <c r="B127" s="4"/>
       <c r="C127" s="4" t="s">
@@ -6922,79 +6800,79 @@
     </row>
     <row r="128" customFormat="false" ht="44" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A128" s="4" t="s">
-        <v>200</v>
+        <v>194</v>
       </c>
       <c r="B128" s="4"/>
       <c r="C128" s="7" t="s">
-        <v>201</v>
+        <v>195</v>
       </c>
       <c r="D128" s="7" t="s">
-        <v>202</v>
+        <v>196</v>
       </c>
     </row>
     <row r="129" customFormat="false" ht="58.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A129" s="9" t="s">
-        <v>203</v>
+        <v>197</v>
       </c>
       <c r="B129" s="4"/>
       <c r="C129" s="7" t="s">
-        <v>204</v>
+        <v>198</v>
       </c>
       <c r="D129" s="7" t="s">
-        <v>205</v>
+        <v>199</v>
       </c>
     </row>
     <row r="130" customFormat="false" ht="58.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A130" s="9" t="s">
-        <v>206</v>
+        <v>200</v>
       </c>
       <c r="B130" s="4"/>
       <c r="C130" s="7" t="s">
-        <v>207</v>
+        <v>201</v>
       </c>
       <c r="D130" s="7" t="s">
-        <v>208</v>
+        <v>202</v>
       </c>
     </row>
     <row r="131" customFormat="false" ht="58.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A131" s="9" t="s">
-        <v>209</v>
+        <v>203</v>
       </c>
       <c r="B131" s="4"/>
       <c r="C131" s="7" t="s">
-        <v>210</v>
+        <v>204</v>
       </c>
       <c r="D131" s="7" t="s">
-        <v>211</v>
+        <v>205</v>
       </c>
     </row>
     <row r="132" customFormat="false" ht="29.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A132" s="4" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="B132" s="4"/>
       <c r="C132" s="7" t="s">
-        <v>212</v>
+        <v>206</v>
       </c>
       <c r="D132" s="7"/>
     </row>
     <row r="133" customFormat="false" ht="29.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A133" s="4" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="B133" s="4"/>
       <c r="C133" s="7" t="s">
-        <v>213</v>
+        <v>207</v>
       </c>
       <c r="D133" s="7"/>
     </row>
     <row r="135" customFormat="false" ht="29.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A135" s="4" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="B135" s="6"/>
       <c r="C135" s="7" t="s">
-        <v>214</v>
+        <v>208</v>
       </c>
     </row>
     <row r="136" customFormat="false" ht="30" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -7003,11 +6881,11 @@
       </c>
       <c r="B136" s="6"/>
       <c r="C136" s="7" t="s">
-        <v>215</v>
+        <v>209</v>
       </c>
     </row>
   </sheetData>
-  <dataValidations count="12">
+  <dataValidations count="36">
     <dataValidation allowBlank="true" operator="equal" showDropDown="false" showErrorMessage="true" showInputMessage="false" sqref="C2" type="list">
       <formula1>"PUBLIC,PRIVATE,DISPUTED"</formula1>
       <formula2>0</formula2>
@@ -7040,11 +6918,7 @@
       <formula1>"PUBLIC,PRIVATE,DISPUTED"</formula1>
       <formula2>0</formula2>
     </dataValidation>
-    <dataValidation allowBlank="true" operator="equal" showDropDown="false" showErrorMessage="true" showInputMessage="false" sqref="C13:D13 C14" type="none">
-      <formula1>0</formula1>
-      <formula2>0</formula2>
-    </dataValidation>
-    <dataValidation allowBlank="true" operator="equal" showDropDown="false" showErrorMessage="true" showInputMessage="false" sqref="D42:D45 D50 D55" type="none">
+    <dataValidation allowBlank="true" operator="equal" showDropDown="false" showErrorMessage="true" showInputMessage="false" sqref="C14" type="none">
       <formula1>0</formula1>
       <formula2>0</formula2>
     </dataValidation>
@@ -7052,8 +6926,108 @@
       <formula1>0</formula1>
       <formula2>0</formula2>
     </dataValidation>
-    <dataValidation allowBlank="true" operator="equal" showDropDown="false" showErrorMessage="true" showInputMessage="false" sqref="C19:D19" type="none">
-      <formula1>0</formula1>
+    <dataValidation allowBlank="true" operator="equal" showDropDown="false" showErrorMessage="true" showInputMessage="false" sqref="D9:D10" type="list">
+      <formula1>"PUBLIC,PRIVATE,DISPUTED"</formula1>
+      <formula2>0</formula2>
+    </dataValidation>
+    <dataValidation allowBlank="true" operator="equal" showDropDown="false" showErrorMessage="true" showInputMessage="false" sqref="D13:D14" type="list">
+      <formula1>"PUBLIC,PRIVATE,DISPUTED"</formula1>
+      <formula2>0</formula2>
+    </dataValidation>
+    <dataValidation allowBlank="true" operator="equal" showDropDown="false" showErrorMessage="true" showInputMessage="false" sqref="D19" type="list">
+      <formula1>"PUBLIC,PRIVATE,DISPUTED"</formula1>
+      <formula2>0</formula2>
+    </dataValidation>
+    <dataValidation allowBlank="true" operator="equal" showDropDown="false" showErrorMessage="true" showInputMessage="false" sqref="D31" type="list">
+      <formula1>"PUBLIC,PRIVATE,DISPUTED"</formula1>
+      <formula2>0</formula2>
+    </dataValidation>
+    <dataValidation allowBlank="true" operator="equal" showDropDown="false" showErrorMessage="true" showInputMessage="false" sqref="D36:D37" type="list">
+      <formula1>"PUBLIC,PRIVATE,DISPUTED"</formula1>
+      <formula2>0</formula2>
+    </dataValidation>
+    <dataValidation allowBlank="true" operator="equal" showDropDown="false" showErrorMessage="true" showInputMessage="false" sqref="D42:D45" type="list">
+      <formula1>"PUBLIC,PRIVATE,DISPUTED"</formula1>
+      <formula2>0</formula2>
+    </dataValidation>
+    <dataValidation allowBlank="true" operator="equal" showDropDown="false" showErrorMessage="true" showInputMessage="false" sqref="D50" type="list">
+      <formula1>"PUBLIC,PRIVATE,DISPUTED"</formula1>
+      <formula2>0</formula2>
+    </dataValidation>
+    <dataValidation allowBlank="true" operator="equal" showDropDown="false" showErrorMessage="true" showInputMessage="false" sqref="D55" type="list">
+      <formula1>"PUBLIC,PRIVATE,DISPUTED"</formula1>
+      <formula2>0</formula2>
+    </dataValidation>
+    <dataValidation allowBlank="true" operator="equal" showDropDown="false" showErrorMessage="true" showInputMessage="false" sqref="D65" type="list">
+      <formula1>"PUBLIC,PRIVATE,DISPUTED"</formula1>
+      <formula2>0</formula2>
+    </dataValidation>
+    <dataValidation allowBlank="true" operator="equal" showDropDown="false" showErrorMessage="true" showInputMessage="false" sqref="D74" type="list">
+      <formula1>"PUBLIC,PRIVATE,DISPUTED"</formula1>
+      <formula2>0</formula2>
+    </dataValidation>
+    <dataValidation allowBlank="true" operator="equal" showDropDown="false" showErrorMessage="true" showInputMessage="false" sqref="D79" type="list">
+      <formula1>"PUBLIC,PRIVATE,DISPUTED"</formula1>
+      <formula2>0</formula2>
+    </dataValidation>
+    <dataValidation allowBlank="true" operator="equal" showDropDown="false" showErrorMessage="true" showInputMessage="false" sqref="D84:D85" type="list">
+      <formula1>"PUBLIC,PRIVATE,DISPUTED"</formula1>
+      <formula2>0</formula2>
+    </dataValidation>
+    <dataValidation allowBlank="true" operator="equal" showDropDown="false" showErrorMessage="true" showInputMessage="false" sqref="D95" type="list">
+      <formula1>"PUBLIC,PRIVATE,DISPUTED"</formula1>
+      <formula2>0</formula2>
+    </dataValidation>
+    <dataValidation allowBlank="true" operator="equal" showDropDown="false" showErrorMessage="true" showInputMessage="false" sqref="D119" type="list">
+      <formula1>"PUBLIC,PRIVATE,DISPUTED"</formula1>
+      <formula2>0</formula2>
+    </dataValidation>
+    <dataValidation allowBlank="true" operator="equal" showDropDown="false" showErrorMessage="true" showInputMessage="false" sqref="C108:C117" type="list">
+      <formula1>"Yes,No,"</formula1>
+      <formula2>0</formula2>
+    </dataValidation>
+    <dataValidation allowBlank="true" operator="equal" showDropDown="false" showErrorMessage="true" showInputMessage="false" sqref="C90:C93" type="list">
+      <formula1>"Yes,No"</formula1>
+      <formula2>0</formula2>
+    </dataValidation>
+    <dataValidation allowBlank="true" operator="equal" showDropDown="false" showErrorMessage="true" showInputMessage="false" sqref="C84" type="list">
+      <formula1>"Yes,No"</formula1>
+      <formula2>0</formula2>
+    </dataValidation>
+    <dataValidation allowBlank="true" operator="equal" showDropDown="false" showErrorMessage="true" showInputMessage="false" sqref="C79" type="list">
+      <formula1>"Yes,No"</formula1>
+      <formula2>0</formula2>
+    </dataValidation>
+    <dataValidation allowBlank="true" operator="equal" showDropDown="false" showErrorMessage="true" showInputMessage="false" sqref="C70:C72" type="list">
+      <formula1>"Yes,No"</formula1>
+      <formula2>0</formula2>
+    </dataValidation>
+    <dataValidation allowBlank="true" operator="equal" showDropDown="false" showErrorMessage="true" showInputMessage="false" sqref="C60:C63" type="list">
+      <formula1>"Yes,No"</formula1>
+      <formula2>0</formula2>
+    </dataValidation>
+    <dataValidation allowBlank="true" operator="equal" showDropDown="false" showErrorMessage="true" showInputMessage="false" sqref="C36" type="list">
+      <formula1>"Yes,No"</formula1>
+      <formula2>0</formula2>
+    </dataValidation>
+    <dataValidation allowBlank="true" operator="equal" showDropDown="false" showErrorMessage="true" showInputMessage="false" sqref="C24:C29" type="list">
+      <formula1>"Yes,No"</formula1>
+      <formula2>0</formula2>
+    </dataValidation>
+    <dataValidation allowBlank="true" operator="equal" showDropDown="false" showErrorMessage="true" showInputMessage="false" sqref="C13" type="list">
+      <formula1>"Current,Abandoned,Launched"</formula1>
+      <formula2>0</formula2>
+    </dataValidation>
+    <dataValidation allowBlank="true" operator="equal" showDropDown="false" showErrorMessage="true" showInputMessage="false" sqref="C19" type="list">
+      <formula1>"Scoping (e.g. pre-feasibility study to support market mapping and issue identification),Early stage (e.g. beginning a feasibility study),Late stage (e.g. final deal construction and placement),Final negotiations"</formula1>
+      <formula2>0</formula2>
+    </dataValidation>
+    <dataValidation allowBlank="true" operator="equal" showDropDown="false" showErrorMessage="true" showInputMessage="false" sqref="C42" type="list">
+      <formula1>"Q1 - 2022,Q2 - 2022,Q3 - 2022,Q4 - 2022,Q1 - 2023,Q2 - 2023,Don’t Know"</formula1>
+      <formula2>0</formula2>
+    </dataValidation>
+    <dataValidation allowBlank="true" operator="equal" showDropDown="false" showErrorMessage="true" showInputMessage="false" sqref="C43" type="list">
+      <formula1>"0-6 months,6-12 months,12-24 months,&gt;24 months "</formula1>
       <formula2>0</formula2>
     </dataValidation>
   </dataValidations>
@@ -7079,7 +7053,7 @@
   <dimension ref="A3:D16"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="E5" activeCellId="0" sqref="E5"/>
+      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -7090,20 +7064,20 @@
     <row r="3" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="14"/>
       <c r="B3" s="4" t="s">
-        <v>216</v>
+        <v>210</v>
       </c>
       <c r="C3" s="4"/>
       <c r="D3" s="4"/>
     </row>
     <row r="4" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="14" t="s">
-        <v>217</v>
+        <v>211</v>
       </c>
       <c r="B4" s="14" t="s">
-        <v>218</v>
+        <v>212</v>
       </c>
       <c r="C4" s="4" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="D4" s="4" t="s">
         <v>14</v>
@@ -7111,16 +7085,16 @@
     </row>
     <row r="5" customFormat="false" ht="86.55" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="15" t="s">
-        <v>219</v>
+        <v>213</v>
       </c>
       <c r="B5" s="15" t="s">
-        <v>220</v>
+        <v>214</v>
       </c>
       <c r="C5" s="7" t="s">
-        <v>221</v>
+        <v>215</v>
       </c>
       <c r="D5" s="7" t="s">
-        <v>222</v>
+        <v>216</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -7221,7 +7195,7 @@
   <dimension ref="A2:K32"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="D2" activeCellId="0" sqref="D2"/>
+      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -7238,34 +7212,34 @@
   <sheetData>
     <row r="2" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="16" t="s">
-        <v>223</v>
+        <v>217</v>
       </c>
       <c r="B2" s="4" t="s">
         <v>8</v>
       </c>
       <c r="C2" s="4" t="s">
+        <v>218</v>
+      </c>
+      <c r="D2" s="4" t="s">
+        <v>219</v>
+      </c>
+      <c r="E2" s="4" t="s">
+        <v>220</v>
+      </c>
+      <c r="F2" s="4" t="s">
+        <v>221</v>
+      </c>
+      <c r="G2" s="4" t="s">
+        <v>222</v>
+      </c>
+      <c r="H2" s="4" t="s">
+        <v>223</v>
+      </c>
+      <c r="I2" s="4" t="s">
         <v>224</v>
       </c>
-      <c r="D2" s="4" t="s">
-        <v>225</v>
-      </c>
-      <c r="E2" s="4" t="s">
-        <v>226</v>
-      </c>
-      <c r="F2" s="4" t="s">
-        <v>227</v>
-      </c>
-      <c r="G2" s="4" t="s">
-        <v>228</v>
-      </c>
-      <c r="H2" s="4" t="s">
-        <v>229</v>
-      </c>
-      <c r="I2" s="4" t="s">
-        <v>230</v>
-      </c>
       <c r="J2" s="4" t="s">
-        <v>216</v>
+        <v>210</v>
       </c>
       <c r="K2" s="4"/>
     </row>
@@ -7274,7 +7248,7 @@
       <c r="B3" s="4"/>
       <c r="C3" s="4"/>
       <c r="D3" s="4" t="s">
-        <v>231</v>
+        <v>225</v>
       </c>
       <c r="E3" s="4"/>
       <c r="F3" s="4"/>
@@ -7282,7 +7256,7 @@
       <c r="H3" s="4"/>
       <c r="I3" s="4"/>
       <c r="J3" s="4" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="K3" s="4" t="s">
         <v>14</v>
@@ -7290,37 +7264,37 @@
     </row>
     <row r="4" customFormat="false" ht="87" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="17" t="s">
+        <v>226</v>
+      </c>
+      <c r="B4" s="7" t="s">
+        <v>227</v>
+      </c>
+      <c r="C4" s="7" t="s">
+        <v>228</v>
+      </c>
+      <c r="D4" s="7" t="s">
+        <v>229</v>
+      </c>
+      <c r="E4" s="7" t="s">
+        <v>230</v>
+      </c>
+      <c r="F4" s="7" t="s">
+        <v>231</v>
+      </c>
+      <c r="G4" s="7" t="s">
         <v>232</v>
       </c>
-      <c r="B4" s="7" t="s">
+      <c r="H4" s="7" t="s">
         <v>233</v>
       </c>
-      <c r="C4" s="7" t="s">
+      <c r="I4" s="7" t="s">
         <v>234</v>
       </c>
-      <c r="D4" s="7" t="s">
+      <c r="J4" s="7" t="s">
         <v>235</v>
       </c>
-      <c r="E4" s="7" t="s">
+      <c r="K4" s="7" t="s">
         <v>236</v>
-      </c>
-      <c r="F4" s="7" t="s">
-        <v>237</v>
-      </c>
-      <c r="G4" s="7" t="s">
-        <v>238</v>
-      </c>
-      <c r="H4" s="7" t="s">
-        <v>239</v>
-      </c>
-      <c r="I4" s="7" t="s">
-        <v>240</v>
-      </c>
-      <c r="J4" s="7" t="s">
-        <v>241</v>
-      </c>
-      <c r="K4" s="7" t="s">
-        <v>242</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -7727,7 +7701,7 @@
   <dimension ref="A2:L32"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A4" activeCellId="0" sqref="A4"/>
+      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -7749,58 +7723,58 @@
     <row r="2" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="14"/>
       <c r="B2" s="4" t="s">
-        <v>243</v>
+        <v>237</v>
       </c>
       <c r="C2" s="4"/>
       <c r="D2" s="4"/>
       <c r="E2" s="4" t="s">
-        <v>244</v>
+        <v>238</v>
       </c>
       <c r="F2" s="4"/>
       <c r="G2" s="4" t="s">
-        <v>245</v>
+        <v>239</v>
       </c>
       <c r="H2" s="4"/>
       <c r="I2" s="4"/>
       <c r="J2" s="4" t="s">
-        <v>216</v>
+        <v>210</v>
       </c>
       <c r="K2" s="4"/>
       <c r="L2" s="4"/>
     </row>
     <row r="3" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="14" t="s">
-        <v>246</v>
+        <v>240</v>
       </c>
       <c r="B3" s="4" t="s">
         <v>8</v>
       </c>
       <c r="C3" s="4" t="s">
-        <v>247</v>
+        <v>241</v>
       </c>
       <c r="D3" s="4" t="s">
-        <v>248</v>
+        <v>242</v>
       </c>
       <c r="E3" s="4" t="s">
-        <v>249</v>
+        <v>243</v>
       </c>
       <c r="F3" s="4" t="s">
-        <v>250</v>
+        <v>244</v>
       </c>
       <c r="G3" s="4" t="s">
         <v>8</v>
       </c>
       <c r="H3" s="4" t="s">
-        <v>251</v>
+        <v>245</v>
       </c>
       <c r="I3" s="4" t="s">
-        <v>252</v>
+        <v>246</v>
       </c>
       <c r="J3" s="14" t="s">
-        <v>218</v>
+        <v>212</v>
       </c>
       <c r="K3" s="4" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="L3" s="4" t="s">
         <v>14</v>
@@ -7808,40 +7782,40 @@
     </row>
     <row r="4" customFormat="false" ht="129.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="15" t="s">
+        <v>247</v>
+      </c>
+      <c r="B4" s="7" t="s">
+        <v>248</v>
+      </c>
+      <c r="C4" s="7" t="s">
+        <v>249</v>
+      </c>
+      <c r="D4" s="7" t="s">
+        <v>250</v>
+      </c>
+      <c r="E4" s="7" t="s">
+        <v>251</v>
+      </c>
+      <c r="F4" s="7" t="s">
+        <v>252</v>
+      </c>
+      <c r="G4" s="7" t="s">
         <v>253</v>
       </c>
-      <c r="B4" s="7" t="s">
+      <c r="H4" s="7" t="s">
         <v>254</v>
       </c>
-      <c r="C4" s="7" t="s">
+      <c r="I4" s="7" t="s">
         <v>255</v>
       </c>
-      <c r="D4" s="7" t="s">
+      <c r="J4" s="15" t="s">
         <v>256</v>
       </c>
-      <c r="E4" s="7" t="s">
+      <c r="K4" s="7" t="s">
         <v>257</v>
       </c>
-      <c r="F4" s="7" t="s">
+      <c r="L4" s="7" t="s">
         <v>258</v>
-      </c>
-      <c r="G4" s="7" t="s">
-        <v>259</v>
-      </c>
-      <c r="H4" s="7" t="s">
-        <v>260</v>
-      </c>
-      <c r="I4" s="7" t="s">
-        <v>261</v>
-      </c>
-      <c r="J4" s="15" t="s">
-        <v>262</v>
-      </c>
-      <c r="K4" s="7" t="s">
-        <v>263</v>
-      </c>
-      <c r="L4" s="7" t="s">
-        <v>264</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -8281,11 +8255,11 @@
   <sheetData>
     <row r="2" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="1" t="s">
-        <v>223</v>
+        <v>217</v>
       </c>
       <c r="B2" s="1"/>
       <c r="C2" s="1" t="s">
-        <v>265</v>
+        <v>259</v>
       </c>
       <c r="D2" s="1"/>
       <c r="E2" s="1"/>
@@ -8294,7 +8268,7 @@
       </c>
       <c r="G2" s="1"/>
       <c r="H2" s="1" t="s">
-        <v>61</v>
+        <v>57</v>
       </c>
       <c r="I2" s="1"/>
       <c r="J2" s="1"/>
@@ -8306,13 +8280,13 @@
         <v>8</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>266</v>
+        <v>260</v>
       </c>
       <c r="D3" s="1" t="s">
-        <v>267</v>
+        <v>261</v>
       </c>
       <c r="E3" s="1" t="s">
-        <v>53</v>
+        <v>49</v>
       </c>
       <c r="F3" s="1" t="s">
         <v>8</v>
@@ -8321,51 +8295,51 @@
         <v>17</v>
       </c>
       <c r="H3" s="1" t="s">
-        <v>268</v>
+        <v>262</v>
       </c>
       <c r="I3" s="1" t="s">
-        <v>269</v>
+        <v>263</v>
       </c>
       <c r="J3" s="1" t="s">
-        <v>247</v>
+        <v>241</v>
       </c>
       <c r="K3" s="1" t="s">
-        <v>248</v>
+        <v>242</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="114.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="18" t="s">
+        <v>264</v>
+      </c>
+      <c r="B4" s="18" t="s">
+        <v>265</v>
+      </c>
+      <c r="C4" s="18" t="s">
+        <v>266</v>
+      </c>
+      <c r="D4" s="18" t="s">
+        <v>267</v>
+      </c>
+      <c r="E4" s="18" t="s">
+        <v>268</v>
+      </c>
+      <c r="F4" s="18" t="s">
+        <v>269</v>
+      </c>
+      <c r="G4" s="18" t="s">
         <v>270</v>
       </c>
-      <c r="B4" s="18" t="s">
+      <c r="H4" s="18" t="s">
         <v>271</v>
       </c>
-      <c r="C4" s="18" t="s">
+      <c r="I4" s="18" t="s">
         <v>272</v>
       </c>
-      <c r="D4" s="18" t="s">
+      <c r="J4" s="18" t="s">
         <v>273</v>
       </c>
-      <c r="E4" s="18" t="s">
+      <c r="K4" s="18" t="s">
         <v>274</v>
-      </c>
-      <c r="F4" s="18" t="s">
-        <v>275</v>
-      </c>
-      <c r="G4" s="18" t="s">
-        <v>276</v>
-      </c>
-      <c r="H4" s="18" t="s">
-        <v>277</v>
-      </c>
-      <c r="I4" s="18" t="s">
-        <v>278</v>
-      </c>
-      <c r="J4" s="18" t="s">
-        <v>279</v>
-      </c>
-      <c r="K4" s="18" t="s">
-        <v>280</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -8756,7 +8730,7 @@
   <dimension ref="A1:I32"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B4" activeCellId="0" sqref="B4"/>
+      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -8779,39 +8753,39 @@
       <c r="C2" s="4"/>
       <c r="D2" s="4"/>
       <c r="E2" s="4" t="s">
-        <v>281</v>
+        <v>275</v>
       </c>
       <c r="F2" s="4"/>
       <c r="G2" s="4" t="s">
-        <v>216</v>
+        <v>210</v>
       </c>
       <c r="H2" s="4"/>
       <c r="I2" s="4"/>
     </row>
     <row r="3" customFormat="false" ht="29.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="16" t="s">
-        <v>282</v>
+        <v>276</v>
       </c>
       <c r="B3" s="14" t="s">
-        <v>283</v>
+        <v>277</v>
       </c>
       <c r="C3" s="9" t="s">
-        <v>284</v>
+        <v>278</v>
       </c>
       <c r="D3" s="4" t="s">
-        <v>156</v>
+        <v>150</v>
       </c>
       <c r="E3" s="4" t="s">
-        <v>285</v>
+        <v>279</v>
       </c>
       <c r="F3" s="4" t="s">
-        <v>286</v>
+        <v>280</v>
       </c>
       <c r="G3" s="14" t="s">
-        <v>218</v>
+        <v>212</v>
       </c>
       <c r="H3" s="4" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="I3" s="4" t="s">
         <v>14</v>
@@ -8819,31 +8793,31 @@
     </row>
     <row r="4" customFormat="false" ht="114.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="19" t="s">
+        <v>281</v>
+      </c>
+      <c r="B4" s="15" t="s">
+        <v>282</v>
+      </c>
+      <c r="C4" s="7" t="s">
+        <v>283</v>
+      </c>
+      <c r="D4" s="7" t="s">
+        <v>284</v>
+      </c>
+      <c r="E4" s="7" t="s">
+        <v>285</v>
+      </c>
+      <c r="F4" s="7" t="s">
+        <v>286</v>
+      </c>
+      <c r="G4" s="15" t="s">
         <v>287</v>
       </c>
-      <c r="B4" s="15" t="s">
+      <c r="H4" s="7" t="s">
         <v>288</v>
       </c>
-      <c r="C4" s="7" t="s">
+      <c r="I4" s="7" t="s">
         <v>289</v>
-      </c>
-      <c r="D4" s="7" t="s">
-        <v>290</v>
-      </c>
-      <c r="E4" s="7" t="s">
-        <v>291</v>
-      </c>
-      <c r="F4" s="7" t="s">
-        <v>292</v>
-      </c>
-      <c r="G4" s="15" t="s">
-        <v>293</v>
-      </c>
-      <c r="H4" s="7" t="s">
-        <v>294</v>
-      </c>
-      <c r="I4" s="7" t="s">
-        <v>295</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -9187,7 +9161,7 @@
   <dimension ref="A1:N32"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="L1" activeCellId="0" sqref="L1"/>
+      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -9214,7 +9188,7 @@
       <c r="A2" s="14"/>
       <c r="B2" s="4"/>
       <c r="C2" s="4" t="s">
-        <v>296</v>
+        <v>290</v>
       </c>
       <c r="D2" s="4"/>
       <c r="E2" s="4"/>
@@ -9222,55 +9196,55 @@
       <c r="G2" s="4"/>
       <c r="H2" s="4"/>
       <c r="I2" s="4" t="s">
-        <v>297</v>
+        <v>291</v>
       </c>
       <c r="J2" s="4"/>
       <c r="K2" s="4"/>
       <c r="L2" s="4" t="s">
-        <v>216</v>
+        <v>210</v>
       </c>
       <c r="M2" s="4"/>
       <c r="N2" s="4"/>
     </row>
     <row r="3" customFormat="false" ht="29.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="14" t="s">
-        <v>283</v>
+        <v>277</v>
       </c>
       <c r="B3" s="9" t="s">
-        <v>284</v>
+        <v>278</v>
       </c>
       <c r="C3" s="4" t="s">
-        <v>298</v>
+        <v>292</v>
       </c>
       <c r="D3" s="4" t="s">
-        <v>299</v>
+        <v>293</v>
       </c>
       <c r="E3" s="4" t="s">
-        <v>300</v>
+        <v>294</v>
       </c>
       <c r="F3" s="4" t="s">
-        <v>301</v>
+        <v>295</v>
       </c>
       <c r="G3" s="4" t="s">
-        <v>302</v>
+        <v>296</v>
       </c>
       <c r="H3" s="4" t="s">
-        <v>303</v>
+        <v>297</v>
       </c>
       <c r="I3" s="4" t="s">
-        <v>298</v>
+        <v>292</v>
       </c>
       <c r="J3" s="4" t="s">
-        <v>299</v>
+        <v>293</v>
       </c>
       <c r="K3" s="4" t="s">
-        <v>300</v>
+        <v>294</v>
       </c>
       <c r="L3" s="14" t="s">
-        <v>218</v>
+        <v>212</v>
       </c>
       <c r="M3" s="4" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="N3" s="4" t="s">
         <v>14</v>
@@ -9278,46 +9252,46 @@
     </row>
     <row r="4" customFormat="false" ht="129.1" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="15" t="s">
+        <v>298</v>
+      </c>
+      <c r="B4" s="7" t="s">
+        <v>299</v>
+      </c>
+      <c r="C4" s="7" t="s">
+        <v>300</v>
+      </c>
+      <c r="D4" s="7" t="s">
+        <v>301</v>
+      </c>
+      <c r="E4" s="7" t="s">
+        <v>302</v>
+      </c>
+      <c r="F4" s="7" t="s">
+        <v>303</v>
+      </c>
+      <c r="G4" s="7" t="s">
         <v>304</v>
       </c>
-      <c r="B4" s="7" t="s">
+      <c r="H4" s="7" t="s">
         <v>305</v>
       </c>
-      <c r="C4" s="7" t="s">
+      <c r="I4" s="7" t="s">
         <v>306</v>
       </c>
-      <c r="D4" s="7" t="s">
+      <c r="J4" s="7" t="s">
         <v>307</v>
       </c>
-      <c r="E4" s="7" t="s">
+      <c r="K4" s="7" t="s">
         <v>308</v>
       </c>
-      <c r="F4" s="7" t="s">
+      <c r="L4" s="15" t="s">
         <v>309</v>
       </c>
-      <c r="G4" s="7" t="s">
+      <c r="M4" s="7" t="s">
         <v>310</v>
       </c>
-      <c r="H4" s="7" t="s">
+      <c r="N4" s="7" t="s">
         <v>311</v>
-      </c>
-      <c r="I4" s="7" t="s">
-        <v>312</v>
-      </c>
-      <c r="J4" s="7" t="s">
-        <v>313</v>
-      </c>
-      <c r="K4" s="7" t="s">
-        <v>314</v>
-      </c>
-      <c r="L4" s="15" t="s">
-        <v>315</v>
-      </c>
-      <c r="M4" s="7" t="s">
-        <v>316</v>
-      </c>
-      <c r="N4" s="7" t="s">
-        <v>317</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -9806,7 +9780,7 @@
   <dimension ref="A1:R33"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="L21" activeCellId="0" sqref="L21"/>
+      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -9835,7 +9809,7 @@
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C2" s="12"/>
       <c r="K2" s="0" t="s">
-        <v>318</v>
+        <v>312</v>
       </c>
       <c r="L2" s="12"/>
       <c r="N2" s="12"/>
@@ -9846,7 +9820,7 @@
       <c r="B3" s="14"/>
       <c r="C3" s="4"/>
       <c r="D3" s="4" t="s">
-        <v>319</v>
+        <v>313</v>
       </c>
       <c r="E3" s="4"/>
       <c r="F3" s="4"/>
@@ -9855,71 +9829,71 @@
       <c r="I3" s="4"/>
       <c r="J3" s="4"/>
       <c r="K3" s="4" t="s">
-        <v>320</v>
+        <v>314</v>
       </c>
       <c r="L3" s="4"/>
       <c r="M3" s="4"/>
       <c r="N3" s="4" t="s">
-        <v>321</v>
+        <v>315</v>
       </c>
       <c r="O3" s="4"/>
       <c r="P3" s="4" t="s">
-        <v>216</v>
+        <v>210</v>
       </c>
       <c r="Q3" s="4"/>
       <c r="R3" s="4"/>
     </row>
     <row r="4" customFormat="false" ht="29.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="16" t="s">
-        <v>282</v>
+        <v>276</v>
       </c>
       <c r="B4" s="14" t="s">
-        <v>283</v>
+        <v>277</v>
       </c>
       <c r="C4" s="9" t="s">
-        <v>284</v>
+        <v>278</v>
       </c>
       <c r="D4" s="4" t="s">
-        <v>298</v>
+        <v>292</v>
       </c>
       <c r="E4" s="4" t="s">
+        <v>316</v>
+      </c>
+      <c r="F4" s="4" t="s">
+        <v>317</v>
+      </c>
+      <c r="G4" s="4" t="s">
+        <v>318</v>
+      </c>
+      <c r="H4" s="4" t="s">
+        <v>319</v>
+      </c>
+      <c r="I4" s="4" t="s">
+        <v>320</v>
+      </c>
+      <c r="J4" s="4" t="s">
+        <v>321</v>
+      </c>
+      <c r="K4" s="4" t="s">
         <v>322</v>
       </c>
-      <c r="F4" s="4" t="s">
+      <c r="L4" s="9" t="s">
         <v>323</v>
       </c>
-      <c r="G4" s="4" t="s">
+      <c r="M4" s="4" t="s">
         <v>324</v>
       </c>
-      <c r="H4" s="4" t="s">
+      <c r="N4" s="9" t="s">
         <v>325</v>
       </c>
-      <c r="I4" s="4" t="s">
+      <c r="O4" s="4" t="s">
         <v>326</v>
       </c>
-      <c r="J4" s="4" t="s">
-        <v>327</v>
-      </c>
-      <c r="K4" s="4" t="s">
-        <v>328</v>
-      </c>
-      <c r="L4" s="9" t="s">
-        <v>329</v>
-      </c>
-      <c r="M4" s="4" t="s">
-        <v>330</v>
-      </c>
-      <c r="N4" s="9" t="s">
-        <v>331</v>
-      </c>
-      <c r="O4" s="4" t="s">
-        <v>332</v>
-      </c>
       <c r="P4" s="14" t="s">
-        <v>218</v>
+        <v>212</v>
       </c>
       <c r="Q4" s="4" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="R4" s="4" t="s">
         <v>14</v>
@@ -9927,58 +9901,58 @@
     </row>
     <row r="5" customFormat="false" ht="115.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="19" t="s">
+        <v>327</v>
+      </c>
+      <c r="B5" s="15" t="s">
+        <v>328</v>
+      </c>
+      <c r="C5" s="7" t="s">
+        <v>329</v>
+      </c>
+      <c r="D5" s="7" t="s">
+        <v>330</v>
+      </c>
+      <c r="E5" s="7" t="s">
+        <v>331</v>
+      </c>
+      <c r="F5" s="7" t="s">
+        <v>332</v>
+      </c>
+      <c r="G5" s="7" t="s">
         <v>333</v>
       </c>
-      <c r="B5" s="15" t="s">
+      <c r="H5" s="7" t="s">
         <v>334</v>
       </c>
-      <c r="C5" s="7" t="s">
+      <c r="I5" s="7" t="s">
         <v>335</v>
       </c>
-      <c r="D5" s="7" t="s">
+      <c r="J5" s="7" t="s">
         <v>336</v>
       </c>
-      <c r="E5" s="7" t="s">
+      <c r="K5" s="7" t="s">
         <v>337</v>
       </c>
-      <c r="F5" s="7" t="s">
+      <c r="L5" s="7" t="s">
         <v>338</v>
       </c>
-      <c r="G5" s="7" t="s">
+      <c r="M5" s="7" t="s">
         <v>339</v>
       </c>
-      <c r="H5" s="7" t="s">
+      <c r="N5" s="7" t="s">
         <v>340</v>
       </c>
-      <c r="I5" s="7" t="s">
+      <c r="O5" s="7" t="s">
         <v>341</v>
       </c>
-      <c r="J5" s="7" t="s">
+      <c r="P5" s="15" t="s">
         <v>342</v>
       </c>
-      <c r="K5" s="7" t="s">
+      <c r="Q5" s="7" t="s">
         <v>343</v>
       </c>
-      <c r="L5" s="7" t="s">
+      <c r="R5" s="7" t="s">
         <v>344</v>
-      </c>
-      <c r="M5" s="7" t="s">
-        <v>345</v>
-      </c>
-      <c r="N5" s="7" t="s">
-        <v>346</v>
-      </c>
-      <c r="O5" s="7" t="s">
-        <v>347</v>
-      </c>
-      <c r="P5" s="15" t="s">
-        <v>348</v>
-      </c>
-      <c r="Q5" s="7" t="s">
-        <v>349</v>
-      </c>
-      <c r="R5" s="7" t="s">
-        <v>350</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">

</xml_diff>

<commit_message>
pipeline: Fix Validity error in Excel
Excel was complaining about a validity error and removing the content.

It was the status column in the "Outcome Payment Commitments" tab.

Not sure what problem was - deleting column and recreating by hand
fixed it.
</commit_message>
<xml_diff>
--- a/indigo/spreadsheetform_guides/pipeline_v001.xlsx
+++ b/indigo/spreadsheetform_guides/pipeline_v001.xlsx
@@ -9262,8 +9262,8 @@
   </sheetPr>
   <dimension ref="A1:N32"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="B1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="B1" activeCellId="0" sqref="B1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -9308,7 +9308,7 @@
       <c r="M2" s="4"/>
       <c r="N2" s="4"/>
     </row>
-    <row r="3" customFormat="false" ht="29.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="3" customFormat="false" ht="30" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="14" t="s">
         <v>287</v>
       </c>
@@ -9352,7 +9352,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="4" customFormat="false" ht="129.1" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="4" customFormat="false" ht="129.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="15" t="s">
         <v>308</v>
       </c>
@@ -9851,16 +9851,16 @@
     <mergeCell ref="L2:N2"/>
   </mergeCells>
   <dataValidations count="3">
-    <dataValidation allowBlank="true" operator="equal" showDropDown="false" showErrorMessage="true" showInputMessage="false" sqref="N4:N32" type="list">
-      <formula1>"PUBLIC,PRIVATE,DISPUTED"</formula1>
-      <formula2>c</formula2>
-    </dataValidation>
     <dataValidation allowBlank="true" operator="equal" showDropDown="false" showErrorMessage="true" showInputMessage="false" sqref="B4:B32" type="list">
       <formula1>"Nonprofit/NGO,Foundation/Philanthropist,Government/Public Sector/Public Bank,Multilateral/Bilateral/Intergovernmental Financial Institution,Corporate Giving,Investment Fund,Other"</formula1>
       <formula2>0</formula2>
     </dataValidation>
     <dataValidation allowBlank="true" operator="equal" showDropDown="false" showErrorMessage="true" showInputMessage="false" sqref="F4:F32" type="list">
       <formula1>"Interim,Overall"</formula1>
+      <formula2>0</formula2>
+    </dataValidation>
+    <dataValidation allowBlank="true" operator="equal" showDropDown="false" showErrorMessage="true" showInputMessage="false" sqref="N4:N32" type="list">
+      <formula1>"PUBLIC,PRIVATE,DISPUTED"</formula1>
       <formula2>0</formula2>
     </dataValidation>
   </dataValidations>

</xml_diff>